<commit_message>
changes from re-running added text analysis on new dataset
</commit_message>
<xml_diff>
--- a/nlp/gen_by_prov.xlsx
+++ b/nlp/gen_by_prov.xlsx
@@ -217,15 +217,18 @@
     <t>щепетильный товар</t>
   </si>
   <si>
+    <t>внутренний товар</t>
+  </si>
+  <si>
+    <t>суровский товар</t>
+  </si>
+  <si>
+    <t>недорогой товар</t>
+  </si>
+  <si>
     <t>питейный припасы</t>
   </si>
   <si>
-    <t>внутренний товар</t>
-  </si>
-  <si>
-    <t>недорогой товар</t>
-  </si>
-  <si>
     <t>медный товар</t>
   </si>
   <si>
@@ -235,9 +238,6 @@
     <t>оловянный товар</t>
   </si>
   <si>
-    <t>суровский товар</t>
-  </si>
-  <si>
     <t>произрастание</t>
   </si>
   <si>
@@ -250,13 +250,13 @@
     <t>галантерейный товар</t>
   </si>
   <si>
+    <t>меховой товар</t>
+  </si>
+  <si>
+    <t>рукодельный товар</t>
+  </si>
+  <si>
     <t>надлежащий товар</t>
-  </si>
-  <si>
-    <t>меховой товар</t>
-  </si>
-  <si>
-    <t>рукодельный товар</t>
   </si>
   <si>
     <t>харчевой припасы</t>
@@ -849,7 +849,7 @@
         <v>24</v>
       </c>
       <c r="AL2" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AM2" s="2">
         <v>17</v>
@@ -861,7 +861,7 @@
         <v>4</v>
       </c>
       <c r="AP2" s="2">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="3" spans="1:42">
@@ -1419,7 +1419,7 @@
         <v>1</v>
       </c>
       <c r="N9" s="2">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="O9" s="2"/>
       <c r="P9" s="2">
@@ -1471,7 +1471,7 @@
         <v>2</v>
       </c>
       <c r="AP9" s="2">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:42">
@@ -2557,9 +2557,7 @@
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
-      <c r="I28" s="2">
-        <v>1</v>
-      </c>
+      <c r="I28" s="2"/>
       <c r="J28" s="2"/>
       <c r="K28" s="2"/>
       <c r="L28" s="2"/>
@@ -2580,21 +2578,25 @@
       <c r="Y28" s="2"/>
       <c r="Z28" s="2"/>
       <c r="AA28" s="2"/>
-      <c r="AB28" s="2"/>
+      <c r="AB28" s="2">
+        <v>1</v>
+      </c>
       <c r="AC28" s="2"/>
       <c r="AD28" s="2"/>
       <c r="AE28" s="2"/>
       <c r="AF28" s="2"/>
       <c r="AG28" s="2"/>
-      <c r="AH28" s="2"/>
+      <c r="AH28" s="2">
+        <v>1</v>
+      </c>
       <c r="AI28" s="2"/>
       <c r="AJ28" s="2"/>
       <c r="AK28" s="2"/>
       <c r="AL28" s="2"/>
-      <c r="AM28" s="2"/>
-      <c r="AN28" s="2">
-        <v>2</v>
-      </c>
+      <c r="AM28" s="2">
+        <v>1</v>
+      </c>
+      <c r="AN28" s="2"/>
       <c r="AO28" s="2"/>
       <c r="AP28" s="2">
         <v>4</v>
@@ -2616,9 +2618,7 @@
       <c r="K29" s="2"/>
       <c r="L29" s="2"/>
       <c r="M29" s="2"/>
-      <c r="N29" s="2">
-        <v>1</v>
-      </c>
+      <c r="N29" s="2"/>
       <c r="O29" s="2"/>
       <c r="P29" s="2"/>
       <c r="Q29" s="2"/>
@@ -2632,26 +2632,22 @@
       <c r="Y29" s="2"/>
       <c r="Z29" s="2"/>
       <c r="AA29" s="2"/>
-      <c r="AB29" s="2">
-        <v>1</v>
-      </c>
+      <c r="AB29" s="2"/>
       <c r="AC29" s="2"/>
       <c r="AD29" s="2"/>
       <c r="AE29" s="2"/>
       <c r="AF29" s="2"/>
       <c r="AG29" s="2"/>
-      <c r="AH29" s="2">
-        <v>1</v>
-      </c>
+      <c r="AH29" s="2"/>
       <c r="AI29" s="2"/>
       <c r="AJ29" s="2"/>
       <c r="AK29" s="2"/>
       <c r="AL29" s="2"/>
-      <c r="AM29" s="2">
-        <v>1</v>
-      </c>
+      <c r="AM29" s="2"/>
       <c r="AN29" s="2"/>
-      <c r="AO29" s="2"/>
+      <c r="AO29" s="2">
+        <v>4</v>
+      </c>
       <c r="AP29" s="2">
         <v>4</v>
       </c>
@@ -2719,14 +2715,16 @@
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
-      <c r="I31" s="2"/>
+      <c r="I31" s="2">
+        <v>1</v>
+      </c>
       <c r="J31" s="2"/>
       <c r="K31" s="2"/>
-      <c r="L31" s="2">
-        <v>1</v>
-      </c>
+      <c r="L31" s="2"/>
       <c r="M31" s="2"/>
-      <c r="N31" s="2"/>
+      <c r="N31" s="2">
+        <v>1</v>
+      </c>
       <c r="O31" s="2"/>
       <c r="P31" s="2"/>
       <c r="Q31" s="2"/>
@@ -2747,9 +2745,7 @@
       <c r="AF31" s="2"/>
       <c r="AG31" s="2"/>
       <c r="AH31" s="2"/>
-      <c r="AI31" s="2">
-        <v>1</v>
-      </c>
+      <c r="AI31" s="2"/>
       <c r="AJ31" s="2"/>
       <c r="AK31" s="2"/>
       <c r="AL31" s="2"/>
@@ -2776,15 +2772,15 @@
       <c r="I32" s="2"/>
       <c r="J32" s="2"/>
       <c r="K32" s="2"/>
-      <c r="L32" s="2"/>
+      <c r="L32" s="2">
+        <v>1</v>
+      </c>
       <c r="M32" s="2"/>
       <c r="N32" s="2"/>
       <c r="O32" s="2"/>
       <c r="P32" s="2"/>
       <c r="Q32" s="2"/>
-      <c r="R32" s="2">
-        <v>1</v>
-      </c>
+      <c r="R32" s="2"/>
       <c r="S32" s="2"/>
       <c r="T32" s="2"/>
       <c r="U32" s="2"/>
@@ -2797,23 +2793,23 @@
       <c r="AB32" s="2"/>
       <c r="AC32" s="2"/>
       <c r="AD32" s="2"/>
-      <c r="AE32" s="2">
-        <v>1</v>
-      </c>
+      <c r="AE32" s="2"/>
       <c r="AF32" s="2"/>
       <c r="AG32" s="2"/>
       <c r="AH32" s="2"/>
-      <c r="AI32" s="2"/>
+      <c r="AI32" s="2">
+        <v>1</v>
+      </c>
       <c r="AJ32" s="2"/>
       <c r="AK32" s="2"/>
       <c r="AL32" s="2"/>
       <c r="AM32" s="2"/>
       <c r="AN32" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AO32" s="2"/>
       <c r="AP32" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="33" spans="1:42">
@@ -2833,12 +2829,12 @@
       <c r="L33" s="2"/>
       <c r="M33" s="2"/>
       <c r="N33" s="2"/>
-      <c r="O33" s="2">
-        <v>1</v>
-      </c>
+      <c r="O33" s="2"/>
       <c r="P33" s="2"/>
       <c r="Q33" s="2"/>
-      <c r="R33" s="2"/>
+      <c r="R33" s="2">
+        <v>1</v>
+      </c>
       <c r="S33" s="2"/>
       <c r="T33" s="2"/>
       <c r="U33" s="2"/>
@@ -2851,13 +2847,13 @@
       <c r="AB33" s="2"/>
       <c r="AC33" s="2"/>
       <c r="AD33" s="2"/>
-      <c r="AE33" s="2"/>
+      <c r="AE33" s="2">
+        <v>1</v>
+      </c>
       <c r="AF33" s="2"/>
       <c r="AG33" s="2"/>
       <c r="AH33" s="2"/>
-      <c r="AI33" s="2">
-        <v>1</v>
-      </c>
+      <c r="AI33" s="2"/>
       <c r="AJ33" s="2"/>
       <c r="AK33" s="2"/>
       <c r="AL33" s="2"/>
@@ -2887,7 +2883,9 @@
       <c r="L34" s="2"/>
       <c r="M34" s="2"/>
       <c r="N34" s="2"/>
-      <c r="O34" s="2"/>
+      <c r="O34" s="2">
+        <v>1</v>
+      </c>
       <c r="P34" s="2"/>
       <c r="Q34" s="2"/>
       <c r="R34" s="2"/>
@@ -2907,15 +2905,17 @@
       <c r="AF34" s="2"/>
       <c r="AG34" s="2"/>
       <c r="AH34" s="2"/>
-      <c r="AI34" s="2"/>
+      <c r="AI34" s="2">
+        <v>1</v>
+      </c>
       <c r="AJ34" s="2"/>
       <c r="AK34" s="2"/>
       <c r="AL34" s="2"/>
       <c r="AM34" s="2"/>
-      <c r="AN34" s="2"/>
-      <c r="AO34" s="2">
-        <v>3</v>
-      </c>
+      <c r="AN34" s="2">
+        <v>1</v>
+      </c>
+      <c r="AO34" s="2"/>
       <c r="AP34" s="2">
         <v>3</v>
       </c>
@@ -3146,7 +3146,9 @@
       <c r="O39" s="2"/>
       <c r="P39" s="2"/>
       <c r="Q39" s="2"/>
-      <c r="R39" s="2"/>
+      <c r="R39" s="2">
+        <v>1</v>
+      </c>
       <c r="S39" s="2"/>
       <c r="T39" s="2"/>
       <c r="U39" s="2"/>
@@ -3165,9 +3167,7 @@
       <c r="AH39" s="2"/>
       <c r="AI39" s="2"/>
       <c r="AJ39" s="2"/>
-      <c r="AK39" s="2">
-        <v>1</v>
-      </c>
+      <c r="AK39" s="2"/>
       <c r="AL39" s="2"/>
       <c r="AM39" s="2"/>
       <c r="AN39" s="2"/>
@@ -3196,9 +3196,7 @@
       <c r="O40" s="2"/>
       <c r="P40" s="2"/>
       <c r="Q40" s="2"/>
-      <c r="R40" s="2">
-        <v>1</v>
-      </c>
+      <c r="R40" s="2"/>
       <c r="S40" s="2"/>
       <c r="T40" s="2"/>
       <c r="U40" s="2"/>
@@ -3220,7 +3218,9 @@
       <c r="AK40" s="2"/>
       <c r="AL40" s="2"/>
       <c r="AM40" s="2"/>
-      <c r="AN40" s="2"/>
+      <c r="AN40" s="2">
+        <v>1</v>
+      </c>
       <c r="AO40" s="2"/>
       <c r="AP40" s="2">
         <v>1</v>
@@ -3265,12 +3265,12 @@
       <c r="AH41" s="2"/>
       <c r="AI41" s="2"/>
       <c r="AJ41" s="2"/>
-      <c r="AK41" s="2"/>
+      <c r="AK41" s="2">
+        <v>1</v>
+      </c>
       <c r="AL41" s="2"/>
       <c r="AM41" s="2"/>
-      <c r="AN41" s="2">
-        <v>1</v>
-      </c>
+      <c r="AN41" s="2"/>
       <c r="AO41" s="2"/>
       <c r="AP41" s="2">
         <v>1</v>

</xml_diff>

<commit_message>
reran adv text processing on new data
</commit_message>
<xml_diff>
--- a/nlp/gen_by_prov.xlsx
+++ b/nlp/gen_by_prov.xlsx
@@ -757,7 +757,7 @@
         <v>41</v>
       </c>
       <c r="B2" s="2">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C2" s="2">
         <v>2</v>
@@ -805,7 +805,7 @@
         <v>2</v>
       </c>
       <c r="T2" s="2">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="U2" s="2"/>
       <c r="V2" s="2"/>
@@ -869,7 +869,7 @@
         <v>42</v>
       </c>
       <c r="B3" s="2">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C3" s="2">
         <v>1</v>
@@ -912,7 +912,9 @@
       <c r="S3" s="2">
         <v>1</v>
       </c>
-      <c r="T3" s="2"/>
+      <c r="T3" s="2">
+        <v>1</v>
+      </c>
       <c r="U3" s="2">
         <v>1</v>
       </c>
@@ -940,7 +942,7 @@
         <v>3</v>
       </c>
       <c r="AE3" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AF3" s="2"/>
       <c r="AG3" s="2"/>
@@ -1162,9 +1164,7 @@
       <c r="A6" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B6" s="2">
-        <v>1</v>
-      </c>
+      <c r="B6" s="2"/>
       <c r="C6" s="2">
         <v>2</v>
       </c>
@@ -1196,7 +1196,9 @@
       <c r="S6" s="2">
         <v>1</v>
       </c>
-      <c r="T6" s="2"/>
+      <c r="T6" s="2">
+        <v>1</v>
+      </c>
       <c r="U6" s="2"/>
       <c r="V6" s="2"/>
       <c r="W6" s="2"/>
@@ -1398,9 +1400,7 @@
       <c r="A9" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B9" s="2">
-        <v>1</v>
-      </c>
+      <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2">
         <v>2</v>
@@ -1430,7 +1430,9 @@
         <v>2</v>
       </c>
       <c r="S9" s="2"/>
-      <c r="T9" s="2"/>
+      <c r="T9" s="2">
+        <v>1</v>
+      </c>
       <c r="U9" s="2">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
added csv output for goods aggregations
</commit_message>
<xml_diff>
--- a/nlp/gen_by_prov.xlsx
+++ b/nlp/gen_by_prov.xlsx
@@ -16,124 +16,124 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="83">
   <si>
+    <t>Ярославское Наместничество</t>
+  </si>
+  <si>
+    <t>Черниговское Наместничество</t>
+  </si>
+  <si>
+    <t>Харьковское Наместничество</t>
+  </si>
+  <si>
+    <t>Уфимское Наместничество</t>
+  </si>
+  <si>
+    <t>Тульское Наместничество</t>
+  </si>
+  <si>
+    <t>Тобольское Наместничество</t>
+  </si>
+  <si>
+    <t>Тверское Наместничество</t>
+  </si>
+  <si>
+    <t>Тамбовское Наместничество</t>
+  </si>
+  <si>
+    <t>Ст Петербургская Губерния</t>
+  </si>
+  <si>
+    <t>Смоленское Наместничество</t>
+  </si>
+  <si>
+    <t>Синбирское Наместничество</t>
+  </si>
+  <si>
+    <t>Саратовское Наместничество</t>
+  </si>
+  <si>
+    <t>Рязанское Наместничество</t>
+  </si>
+  <si>
+    <t>Рижское Наместничество</t>
+  </si>
+  <si>
+    <t>Псковское Наместничество</t>
+  </si>
+  <si>
+    <t>Полотское Наместничество</t>
+  </si>
+  <si>
+    <t>Пермское Наместничество</t>
+  </si>
+  <si>
+    <t>Пензенское Наместничество</t>
+  </si>
+  <si>
+    <t>Орловское Наместничество</t>
+  </si>
+  <si>
+    <t>Олонецкое Наместничество</t>
+  </si>
+  <si>
+    <t>Новогородское Наместничество</t>
+  </si>
+  <si>
+    <t>Новогород - Северское Наместничество</t>
+  </si>
+  <si>
+    <t>Нижегородское Наместничество</t>
+  </si>
+  <si>
+    <t>Московская Губерния</t>
+  </si>
+  <si>
+    <t>Могилевское Наместничество</t>
+  </si>
+  <si>
+    <t>Курское Наместничество</t>
+  </si>
+  <si>
+    <t>Костромское Наместничество</t>
+  </si>
+  <si>
+    <t>Киевское Наместничество</t>
+  </si>
+  <si>
+    <t>Калужское Наместничество</t>
+  </si>
+  <si>
+    <t>Казанское Наместничество</t>
+  </si>
+  <si>
+    <t>Кавказское Наместничество</t>
+  </si>
+  <si>
+    <t>Иркутское Наместничество</t>
+  </si>
+  <si>
+    <t>Екатеринославское Наместничество</t>
+  </si>
+  <si>
+    <t>Вятское Наместничество</t>
+  </si>
+  <si>
+    <t>Выборгское Наместничество</t>
+  </si>
+  <si>
+    <t>Воронежское Наместничество</t>
+  </si>
+  <si>
+    <t>Вологодское Наместничество</t>
+  </si>
+  <si>
+    <t>Владимерское Наместничество</t>
+  </si>
+  <si>
+    <t>Архангельское Наместничество</t>
+  </si>
+  <si>
     <t>None</t>
-  </si>
-  <si>
-    <t>Архангельское Наместничество</t>
-  </si>
-  <si>
-    <t>Владимерское Наместничество</t>
-  </si>
-  <si>
-    <t>Вологодское Наместничество</t>
-  </si>
-  <si>
-    <t>Воронежское Наместничество</t>
-  </si>
-  <si>
-    <t>Выборгское Наместничество</t>
-  </si>
-  <si>
-    <t>Вятское Наместничество</t>
-  </si>
-  <si>
-    <t>Екатеринославское Наместничество</t>
-  </si>
-  <si>
-    <t>Иркутское Наместничество</t>
-  </si>
-  <si>
-    <t>Кавказское Наместничество</t>
-  </si>
-  <si>
-    <t>Казанское Наместничество</t>
-  </si>
-  <si>
-    <t>Калужское Наместничество</t>
-  </si>
-  <si>
-    <t>Киевское Наместничество</t>
-  </si>
-  <si>
-    <t>Костромское Наместничество</t>
-  </si>
-  <si>
-    <t>Курское Наместничество</t>
-  </si>
-  <si>
-    <t>Могилевское Наместничество</t>
-  </si>
-  <si>
-    <t>Московская Губерния</t>
-  </si>
-  <si>
-    <t>Нижегородское Наместничество</t>
-  </si>
-  <si>
-    <t>Новогород - Северское Наместничество</t>
-  </si>
-  <si>
-    <t>Новогородское Наместничество</t>
-  </si>
-  <si>
-    <t>Олонецкое Наместничество</t>
-  </si>
-  <si>
-    <t>Орловское Наместничество</t>
-  </si>
-  <si>
-    <t>Пензенское Наместничество</t>
-  </si>
-  <si>
-    <t>Пермское Наместничество</t>
-  </si>
-  <si>
-    <t>Полотское Наместничество</t>
-  </si>
-  <si>
-    <t>Псковское Наместничество</t>
-  </si>
-  <si>
-    <t>Рижское Наместничество</t>
-  </si>
-  <si>
-    <t>Рязанское Наместничество</t>
-  </si>
-  <si>
-    <t>Саратовское Наместничество</t>
-  </si>
-  <si>
-    <t>Синбирское Наместничество</t>
-  </si>
-  <si>
-    <t>Смоленское Наместничество</t>
-  </si>
-  <si>
-    <t>Ст Петербургская Губерния</t>
-  </si>
-  <si>
-    <t>Тамбовское Наместничество</t>
-  </si>
-  <si>
-    <t>Тверское Наместничество</t>
-  </si>
-  <si>
-    <t>Тобольское Наместничество</t>
-  </si>
-  <si>
-    <t>Тульское Наместничество</t>
-  </si>
-  <si>
-    <t>Уфимское Наместничество</t>
-  </si>
-  <si>
-    <t>Харьковское Наместничество</t>
-  </si>
-  <si>
-    <t>Черниговское Наместничество</t>
-  </si>
-  <si>
-    <t>Ярославское Наместничество</t>
   </si>
   <si>
     <t>Total</t>
@@ -757,124 +757,124 @@
         <v>41</v>
       </c>
       <c r="B2" s="2">
+        <v>4</v>
+      </c>
+      <c r="C2" s="2">
+        <v>12</v>
+      </c>
+      <c r="D2" s="2">
+        <v>17</v>
+      </c>
+      <c r="E2" s="2">
+        <v>5</v>
+      </c>
+      <c r="F2" s="2">
+        <v>24</v>
+      </c>
+      <c r="G2" s="2">
+        <v>1</v>
+      </c>
+      <c r="H2" s="2">
+        <v>17</v>
+      </c>
+      <c r="I2" s="2">
+        <v>18</v>
+      </c>
+      <c r="J2" s="2">
+        <v>0</v>
+      </c>
+      <c r="K2" s="2">
+        <v>0</v>
+      </c>
+      <c r="L2" s="2">
+        <v>2</v>
+      </c>
+      <c r="M2" s="2">
+        <v>2</v>
+      </c>
+      <c r="N2" s="2">
+        <v>9</v>
+      </c>
+      <c r="O2" s="2">
+        <v>0</v>
+      </c>
+      <c r="P2" s="2">
+        <v>11</v>
+      </c>
+      <c r="Q2" s="2">
+        <v>27</v>
+      </c>
+      <c r="R2" s="2">
+        <v>2</v>
+      </c>
+      <c r="S2" s="2">
+        <v>10</v>
+      </c>
+      <c r="T2" s="2">
+        <v>10</v>
+      </c>
+      <c r="U2" s="2">
+        <v>0</v>
+      </c>
+      <c r="V2" s="2">
+        <v>0</v>
+      </c>
+      <c r="W2" s="2">
+        <v>9</v>
+      </c>
+      <c r="X2" s="2">
+        <v>2</v>
+      </c>
+      <c r="Y2" s="2">
+        <v>10</v>
+      </c>
+      <c r="Z2" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA2" s="2">
+        <v>2</v>
+      </c>
+      <c r="AB2" s="2">
         <v>7</v>
       </c>
-      <c r="C2" s="2">
+      <c r="AC2" s="2">
+        <v>23</v>
+      </c>
+      <c r="AD2" s="2">
+        <v>7</v>
+      </c>
+      <c r="AE2" s="2">
+        <v>3</v>
+      </c>
+      <c r="AF2" s="2">
+        <v>0</v>
+      </c>
+      <c r="AG2" s="2">
         <v>2</v>
       </c>
-      <c r="D2" s="2">
+      <c r="AH2" s="2">
+        <v>2</v>
+      </c>
+      <c r="AI2" s="2">
+        <v>2</v>
+      </c>
+      <c r="AJ2" s="2">
+        <v>0</v>
+      </c>
+      <c r="AK2" s="2">
+        <v>2</v>
+      </c>
+      <c r="AL2" s="2">
+        <v>11</v>
+      </c>
+      <c r="AM2" s="2">
         <v>9</v>
       </c>
-      <c r="E2" s="2">
-        <v>11</v>
-      </c>
-      <c r="F2" s="2">
+      <c r="AN2" s="2">
         <v>2</v>
       </c>
-      <c r="G2" s="2">
-        <v>0</v>
-      </c>
-      <c r="H2" s="2">
-        <v>2</v>
-      </c>
-      <c r="I2" s="2">
-        <v>2</v>
-      </c>
-      <c r="J2" s="2">
-        <v>2</v>
-      </c>
-      <c r="K2" s="2">
-        <v>0</v>
-      </c>
-      <c r="L2" s="2">
-        <v>3</v>
-      </c>
-      <c r="M2" s="2">
+      <c r="AO2" s="2">
         <v>7</v>
-      </c>
-      <c r="N2" s="2">
-        <v>23</v>
-      </c>
-      <c r="O2" s="2">
-        <v>7</v>
-      </c>
-      <c r="P2" s="2">
-        <v>2</v>
-      </c>
-      <c r="Q2" s="2">
-        <v>0</v>
-      </c>
-      <c r="R2" s="2">
-        <v>10</v>
-      </c>
-      <c r="S2" s="2">
-        <v>2</v>
-      </c>
-      <c r="T2" s="2">
-        <v>9</v>
-      </c>
-      <c r="U2" s="2">
-        <v>0</v>
-      </c>
-      <c r="V2" s="2">
-        <v>0</v>
-      </c>
-      <c r="W2" s="2">
-        <v>10</v>
-      </c>
-      <c r="X2" s="2">
-        <v>10</v>
-      </c>
-      <c r="Y2" s="2">
-        <v>2</v>
-      </c>
-      <c r="Z2" s="2">
-        <v>27</v>
-      </c>
-      <c r="AA2" s="2">
-        <v>11</v>
-      </c>
-      <c r="AB2" s="2">
-        <v>0</v>
-      </c>
-      <c r="AC2" s="2">
-        <v>9</v>
-      </c>
-      <c r="AD2" s="2">
-        <v>2</v>
-      </c>
-      <c r="AE2" s="2">
-        <v>2</v>
-      </c>
-      <c r="AF2" s="2">
-        <v>0</v>
-      </c>
-      <c r="AG2" s="2">
-        <v>0</v>
-      </c>
-      <c r="AH2" s="2">
-        <v>18</v>
-      </c>
-      <c r="AI2" s="2">
-        <v>17</v>
-      </c>
-      <c r="AJ2" s="2">
-        <v>1</v>
-      </c>
-      <c r="AK2" s="2">
-        <v>24</v>
-      </c>
-      <c r="AL2" s="2">
-        <v>5</v>
-      </c>
-      <c r="AM2" s="2">
-        <v>17</v>
-      </c>
-      <c r="AN2" s="2">
-        <v>12</v>
-      </c>
-      <c r="AO2" s="2">
-        <v>4</v>
       </c>
       <c r="AP2" s="2">
         <v>271</v>
@@ -885,124 +885,124 @@
         <v>42</v>
       </c>
       <c r="B3" s="2">
+        <v>4</v>
+      </c>
+      <c r="C3" s="2">
+        <v>3</v>
+      </c>
+      <c r="D3" s="2">
+        <v>24</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0</v>
+      </c>
+      <c r="F3" s="2">
+        <v>1</v>
+      </c>
+      <c r="G3" s="2">
+        <v>0</v>
+      </c>
+      <c r="H3" s="2">
+        <v>7</v>
+      </c>
+      <c r="I3" s="2">
+        <v>8</v>
+      </c>
+      <c r="J3" s="2">
+        <v>0</v>
+      </c>
+      <c r="K3" s="2">
+        <v>0</v>
+      </c>
+      <c r="L3" s="2">
+        <v>6</v>
+      </c>
+      <c r="M3" s="2">
+        <v>3</v>
+      </c>
+      <c r="N3" s="2">
+        <v>2</v>
+      </c>
+      <c r="O3" s="2">
+        <v>2</v>
+      </c>
+      <c r="P3" s="2">
+        <v>3</v>
+      </c>
+      <c r="Q3" s="2">
+        <v>0</v>
+      </c>
+      <c r="R3" s="2">
+        <v>0</v>
+      </c>
+      <c r="S3" s="2">
+        <v>6</v>
+      </c>
+      <c r="T3" s="2">
         <v>5</v>
       </c>
-      <c r="C3" s="2">
-        <v>1</v>
-      </c>
-      <c r="D3" s="2">
+      <c r="U3" s="2">
         <v>2</v>
       </c>
-      <c r="E3" s="2">
-        <v>0</v>
-      </c>
-      <c r="F3" s="2">
+      <c r="V3" s="2">
+        <v>1</v>
+      </c>
+      <c r="W3" s="2">
+        <v>1</v>
+      </c>
+      <c r="X3" s="2">
+        <v>1</v>
+      </c>
+      <c r="Y3" s="2">
+        <v>6</v>
+      </c>
+      <c r="Z3" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA3" s="2">
         <v>4</v>
       </c>
-      <c r="G3" s="2">
-        <v>0</v>
-      </c>
-      <c r="H3" s="2">
+      <c r="AB3" s="2">
+        <v>4</v>
+      </c>
+      <c r="AC3" s="2">
+        <v>1</v>
+      </c>
+      <c r="AD3" s="2">
+        <v>10</v>
+      </c>
+      <c r="AE3" s="2">
         <v>2</v>
       </c>
-      <c r="I3" s="2">
-        <v>0</v>
-      </c>
-      <c r="J3" s="2">
-        <v>0</v>
-      </c>
-      <c r="K3" s="2">
-        <v>1</v>
-      </c>
-      <c r="L3" s="2">
+      <c r="AF3" s="2">
+        <v>1</v>
+      </c>
+      <c r="AG3" s="2">
+        <v>0</v>
+      </c>
+      <c r="AH3" s="2">
+        <v>0</v>
+      </c>
+      <c r="AI3" s="2">
         <v>2</v>
       </c>
-      <c r="M3" s="2">
-        <v>10</v>
-      </c>
-      <c r="N3" s="2">
-        <v>1</v>
-      </c>
-      <c r="O3" s="2">
+      <c r="AJ3" s="2">
+        <v>0</v>
+      </c>
+      <c r="AK3" s="2">
         <v>4</v>
       </c>
-      <c r="P3" s="2">
-        <v>4</v>
-      </c>
-      <c r="Q3" s="2">
-        <v>0</v>
-      </c>
-      <c r="R3" s="2">
-        <v>6</v>
-      </c>
-      <c r="S3" s="2">
-        <v>1</v>
-      </c>
-      <c r="T3" s="2">
-        <v>1</v>
-      </c>
-      <c r="U3" s="2">
-        <v>1</v>
-      </c>
-      <c r="V3" s="2">
+      <c r="AL3" s="2">
+        <v>0</v>
+      </c>
+      <c r="AM3" s="2">
         <v>2</v>
       </c>
-      <c r="W3" s="2">
+      <c r="AN3" s="2">
+        <v>1</v>
+      </c>
+      <c r="AO3" s="2">
         <v>5</v>
-      </c>
-      <c r="X3" s="2">
-        <v>6</v>
-      </c>
-      <c r="Y3" s="2">
-        <v>0</v>
-      </c>
-      <c r="Z3" s="2">
-        <v>0</v>
-      </c>
-      <c r="AA3" s="2">
-        <v>3</v>
-      </c>
-      <c r="AB3" s="2">
-        <v>2</v>
-      </c>
-      <c r="AC3" s="2">
-        <v>2</v>
-      </c>
-      <c r="AD3" s="2">
-        <v>3</v>
-      </c>
-      <c r="AE3" s="2">
-        <v>6</v>
-      </c>
-      <c r="AF3" s="2">
-        <v>0</v>
-      </c>
-      <c r="AG3" s="2">
-        <v>0</v>
-      </c>
-      <c r="AH3" s="2">
-        <v>8</v>
-      </c>
-      <c r="AI3" s="2">
-        <v>7</v>
-      </c>
-      <c r="AJ3" s="2">
-        <v>0</v>
-      </c>
-      <c r="AK3" s="2">
-        <v>1</v>
-      </c>
-      <c r="AL3" s="2">
-        <v>0</v>
-      </c>
-      <c r="AM3" s="2">
-        <v>24</v>
-      </c>
-      <c r="AN3" s="2">
-        <v>3</v>
-      </c>
-      <c r="AO3" s="2">
-        <v>4</v>
       </c>
       <c r="AP3" s="2">
         <v>121</v>
@@ -1013,124 +1013,124 @@
         <v>43</v>
       </c>
       <c r="B4" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C4" s="2">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="D4" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E4" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F4" s="2">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G4" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H4" s="2">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="I4" s="2">
         <v>2</v>
       </c>
       <c r="J4" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K4" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L4" s="2">
         <v>1</v>
       </c>
       <c r="M4" s="2">
+        <v>1</v>
+      </c>
+      <c r="N4" s="2">
         <v>2</v>
       </c>
-      <c r="N4" s="2">
+      <c r="O4" s="2">
+        <v>0</v>
+      </c>
+      <c r="P4" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="2">
+        <v>0</v>
+      </c>
+      <c r="R4" s="2">
+        <v>1</v>
+      </c>
+      <c r="S4" s="2">
+        <v>0</v>
+      </c>
+      <c r="T4" s="2">
+        <v>6</v>
+      </c>
+      <c r="U4" s="2">
+        <v>0</v>
+      </c>
+      <c r="V4" s="2">
+        <v>2</v>
+      </c>
+      <c r="W4" s="2">
+        <v>0</v>
+      </c>
+      <c r="X4" s="2">
+        <v>3</v>
+      </c>
+      <c r="Y4" s="2">
         <v>7</v>
       </c>
-      <c r="O4" s="2">
-        <v>1</v>
-      </c>
-      <c r="P4" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="2">
-        <v>0</v>
-      </c>
-      <c r="R4" s="2">
+      <c r="Z4" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA4" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB4" s="2">
+        <v>1</v>
+      </c>
+      <c r="AC4" s="2">
         <v>7</v>
       </c>
-      <c r="S4" s="2">
-        <v>3</v>
-      </c>
-      <c r="T4" s="2">
-        <v>0</v>
-      </c>
-      <c r="U4" s="2">
+      <c r="AD4" s="2">
         <v>2</v>
       </c>
-      <c r="V4" s="2">
-        <v>0</v>
-      </c>
-      <c r="W4" s="2">
-        <v>6</v>
-      </c>
-      <c r="X4" s="2">
-        <v>0</v>
-      </c>
-      <c r="Y4" s="2">
-        <v>1</v>
-      </c>
-      <c r="Z4" s="2">
-        <v>0</v>
-      </c>
-      <c r="AA4" s="2">
-        <v>0</v>
-      </c>
-      <c r="AB4" s="2">
-        <v>0</v>
-      </c>
-      <c r="AC4" s="2">
-        <v>2</v>
-      </c>
-      <c r="AD4" s="2">
-        <v>1</v>
-      </c>
       <c r="AE4" s="2">
         <v>1</v>
       </c>
       <c r="AF4" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG4" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH4" s="2">
         <v>2</v>
       </c>
       <c r="AI4" s="2">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="AJ4" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK4" s="2">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="AL4" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AM4" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AN4" s="2">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="AO4" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AP4" s="2">
         <v>76</v>
@@ -1141,124 +1141,124 @@
         <v>44</v>
       </c>
       <c r="B5" s="2">
+        <v>1</v>
+      </c>
+      <c r="C5" s="2">
+        <v>2</v>
+      </c>
+      <c r="D5" s="2">
+        <v>17</v>
+      </c>
+      <c r="E5" s="2">
+        <v>1</v>
+      </c>
+      <c r="F5" s="2">
+        <v>0</v>
+      </c>
+      <c r="G5" s="2">
+        <v>0</v>
+      </c>
+      <c r="H5" s="2">
+        <v>5</v>
+      </c>
+      <c r="I5" s="2">
+        <v>6</v>
+      </c>
+      <c r="J5" s="2">
+        <v>0</v>
+      </c>
+      <c r="K5" s="2">
+        <v>0</v>
+      </c>
+      <c r="L5" s="2">
+        <v>1</v>
+      </c>
+      <c r="M5" s="2">
+        <v>0</v>
+      </c>
+      <c r="N5" s="2">
+        <v>1</v>
+      </c>
+      <c r="O5" s="2">
+        <v>1</v>
+      </c>
+      <c r="P5" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="2">
+        <v>0</v>
+      </c>
+      <c r="R5" s="2">
+        <v>0</v>
+      </c>
+      <c r="S5" s="2">
+        <v>1</v>
+      </c>
+      <c r="T5" s="2">
+        <v>0</v>
+      </c>
+      <c r="U5" s="2">
+        <v>2</v>
+      </c>
+      <c r="V5" s="2">
+        <v>0</v>
+      </c>
+      <c r="W5" s="2">
+        <v>0</v>
+      </c>
+      <c r="X5" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y5" s="2">
+        <v>2</v>
+      </c>
+      <c r="Z5" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA5" s="2">
+        <v>2</v>
+      </c>
+      <c r="AB5" s="2">
+        <v>1</v>
+      </c>
+      <c r="AC5" s="2">
+        <v>1</v>
+      </c>
+      <c r="AD5" s="2">
+        <v>9</v>
+      </c>
+      <c r="AE5" s="2">
+        <v>1</v>
+      </c>
+      <c r="AF5" s="2">
+        <v>1</v>
+      </c>
+      <c r="AG5" s="2">
+        <v>0</v>
+      </c>
+      <c r="AH5" s="2">
+        <v>0</v>
+      </c>
+      <c r="AI5" s="2">
+        <v>2</v>
+      </c>
+      <c r="AJ5" s="2">
+        <v>0</v>
+      </c>
+      <c r="AK5" s="2">
+        <v>2</v>
+      </c>
+      <c r="AL5" s="2">
+        <v>0</v>
+      </c>
+      <c r="AM5" s="2">
+        <v>1</v>
+      </c>
+      <c r="AN5" s="2">
+        <v>1</v>
+      </c>
+      <c r="AO5" s="2">
         <v>4</v>
-      </c>
-      <c r="C5" s="2">
-        <v>1</v>
-      </c>
-      <c r="D5" s="2">
-        <v>1</v>
-      </c>
-      <c r="E5" s="2">
-        <v>0</v>
-      </c>
-      <c r="F5" s="2">
-        <v>2</v>
-      </c>
-      <c r="G5" s="2">
-        <v>0</v>
-      </c>
-      <c r="H5" s="2">
-        <v>2</v>
-      </c>
-      <c r="I5" s="2">
-        <v>0</v>
-      </c>
-      <c r="J5" s="2">
-        <v>0</v>
-      </c>
-      <c r="K5" s="2">
-        <v>1</v>
-      </c>
-      <c r="L5" s="2">
-        <v>1</v>
-      </c>
-      <c r="M5" s="2">
-        <v>9</v>
-      </c>
-      <c r="N5" s="2">
-        <v>1</v>
-      </c>
-      <c r="O5" s="2">
-        <v>1</v>
-      </c>
-      <c r="P5" s="2">
-        <v>2</v>
-      </c>
-      <c r="Q5" s="2">
-        <v>0</v>
-      </c>
-      <c r="R5" s="2">
-        <v>2</v>
-      </c>
-      <c r="S5" s="2">
-        <v>0</v>
-      </c>
-      <c r="T5" s="2">
-        <v>0</v>
-      </c>
-      <c r="U5" s="2">
-        <v>0</v>
-      </c>
-      <c r="V5" s="2">
-        <v>2</v>
-      </c>
-      <c r="W5" s="2">
-        <v>0</v>
-      </c>
-      <c r="X5" s="2">
-        <v>1</v>
-      </c>
-      <c r="Y5" s="2">
-        <v>0</v>
-      </c>
-      <c r="Z5" s="2">
-        <v>0</v>
-      </c>
-      <c r="AA5" s="2">
-        <v>1</v>
-      </c>
-      <c r="AB5" s="2">
-        <v>1</v>
-      </c>
-      <c r="AC5" s="2">
-        <v>1</v>
-      </c>
-      <c r="AD5" s="2">
-        <v>0</v>
-      </c>
-      <c r="AE5" s="2">
-        <v>1</v>
-      </c>
-      <c r="AF5" s="2">
-        <v>0</v>
-      </c>
-      <c r="AG5" s="2">
-        <v>0</v>
-      </c>
-      <c r="AH5" s="2">
-        <v>6</v>
-      </c>
-      <c r="AI5" s="2">
-        <v>5</v>
-      </c>
-      <c r="AJ5" s="2">
-        <v>0</v>
-      </c>
-      <c r="AK5" s="2">
-        <v>0</v>
-      </c>
-      <c r="AL5" s="2">
-        <v>1</v>
-      </c>
-      <c r="AM5" s="2">
-        <v>17</v>
-      </c>
-      <c r="AN5" s="2">
-        <v>2</v>
-      </c>
-      <c r="AO5" s="2">
-        <v>1</v>
       </c>
       <c r="AP5" s="2">
         <v>66</v>
@@ -1269,124 +1269,124 @@
         <v>45</v>
       </c>
       <c r="B6" s="2">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C6" s="2">
+        <v>8</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0</v>
+      </c>
+      <c r="F6" s="2">
+        <v>8</v>
+      </c>
+      <c r="G6" s="2">
+        <v>0</v>
+      </c>
+      <c r="H6" s="2">
+        <v>1</v>
+      </c>
+      <c r="I6" s="2">
+        <v>1</v>
+      </c>
+      <c r="J6" s="2">
+        <v>0</v>
+      </c>
+      <c r="K6" s="2">
+        <v>0</v>
+      </c>
+      <c r="L6" s="2">
+        <v>0</v>
+      </c>
+      <c r="M6" s="2">
+        <v>0</v>
+      </c>
+      <c r="N6" s="2">
         <v>2</v>
       </c>
-      <c r="D6" s="2">
-        <v>1</v>
-      </c>
-      <c r="E6" s="2">
-        <v>0</v>
-      </c>
-      <c r="F6" s="2">
-        <v>0</v>
-      </c>
-      <c r="G6" s="2">
-        <v>0</v>
-      </c>
-      <c r="H6" s="2">
-        <v>0</v>
-      </c>
-      <c r="I6" s="2">
-        <v>1</v>
-      </c>
-      <c r="J6" s="2">
-        <v>0</v>
-      </c>
-      <c r="K6" s="2">
-        <v>0</v>
-      </c>
-      <c r="L6" s="2">
-        <v>1</v>
-      </c>
-      <c r="M6" s="2">
-        <v>0</v>
-      </c>
-      <c r="N6" s="2">
+      <c r="O6" s="2">
+        <v>1</v>
+      </c>
+      <c r="P6" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="2">
+        <v>0</v>
+      </c>
+      <c r="R6" s="2">
+        <v>1</v>
+      </c>
+      <c r="S6" s="2">
+        <v>0</v>
+      </c>
+      <c r="T6" s="2">
+        <v>0</v>
+      </c>
+      <c r="U6" s="2">
+        <v>0</v>
+      </c>
+      <c r="V6" s="2">
+        <v>0</v>
+      </c>
+      <c r="W6" s="2">
+        <v>1</v>
+      </c>
+      <c r="X6" s="2">
+        <v>1</v>
+      </c>
+      <c r="Y6" s="2">
+        <v>5</v>
+      </c>
+      <c r="Z6" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA6" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB6" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC6" s="2">
         <v>7</v>
       </c>
-      <c r="O6" s="2">
-        <v>0</v>
-      </c>
-      <c r="P6" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q6" s="2">
-        <v>0</v>
-      </c>
-      <c r="R6" s="2">
-        <v>5</v>
-      </c>
-      <c r="S6" s="2">
-        <v>1</v>
-      </c>
-      <c r="T6" s="2">
-        <v>1</v>
-      </c>
-      <c r="U6" s="2">
-        <v>0</v>
-      </c>
-      <c r="V6" s="2">
-        <v>0</v>
-      </c>
-      <c r="W6" s="2">
-        <v>0</v>
-      </c>
-      <c r="X6" s="2">
-        <v>0</v>
-      </c>
-      <c r="Y6" s="2">
-        <v>1</v>
-      </c>
-      <c r="Z6" s="2">
-        <v>0</v>
-      </c>
-      <c r="AA6" s="2">
-        <v>0</v>
-      </c>
-      <c r="AB6" s="2">
-        <v>1</v>
-      </c>
-      <c r="AC6" s="2">
+      <c r="AD6" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE6" s="2">
+        <v>1</v>
+      </c>
+      <c r="AF6" s="2">
+        <v>0</v>
+      </c>
+      <c r="AG6" s="2">
+        <v>0</v>
+      </c>
+      <c r="AH6" s="2">
+        <v>1</v>
+      </c>
+      <c r="AI6" s="2">
+        <v>0</v>
+      </c>
+      <c r="AJ6" s="2">
+        <v>0</v>
+      </c>
+      <c r="AK6" s="2">
+        <v>0</v>
+      </c>
+      <c r="AL6" s="2">
+        <v>0</v>
+      </c>
+      <c r="AM6" s="2">
+        <v>1</v>
+      </c>
+      <c r="AN6" s="2">
         <v>2</v>
       </c>
-      <c r="AD6" s="2">
-        <v>0</v>
-      </c>
-      <c r="AE6" s="2">
-        <v>0</v>
-      </c>
-      <c r="AF6" s="2">
-        <v>0</v>
-      </c>
-      <c r="AG6" s="2">
-        <v>0</v>
-      </c>
-      <c r="AH6" s="2">
-        <v>1</v>
-      </c>
-      <c r="AI6" s="2">
-        <v>1</v>
-      </c>
-      <c r="AJ6" s="2">
-        <v>0</v>
-      </c>
-      <c r="AK6" s="2">
-        <v>8</v>
-      </c>
-      <c r="AL6" s="2">
-        <v>0</v>
-      </c>
-      <c r="AM6" s="2">
-        <v>0</v>
-      </c>
-      <c r="AN6" s="2">
-        <v>8</v>
-      </c>
       <c r="AO6" s="2">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AP6" s="2">
         <v>45</v>
@@ -1400,118 +1400,118 @@
         <v>0</v>
       </c>
       <c r="C7" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D7" s="2">
+        <v>0</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0</v>
+      </c>
+      <c r="F7" s="2">
+        <v>0</v>
+      </c>
+      <c r="G7" s="2">
+        <v>0</v>
+      </c>
+      <c r="H7" s="2">
+        <v>1</v>
+      </c>
+      <c r="I7" s="2">
+        <v>1</v>
+      </c>
+      <c r="J7" s="2">
+        <v>1</v>
+      </c>
+      <c r="K7" s="2">
+        <v>0</v>
+      </c>
+      <c r="L7" s="2">
+        <v>1</v>
+      </c>
+      <c r="M7" s="2">
+        <v>0</v>
+      </c>
+      <c r="N7" s="2">
+        <v>1</v>
+      </c>
+      <c r="O7" s="2">
+        <v>0</v>
+      </c>
+      <c r="P7" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q7" s="2">
+        <v>0</v>
+      </c>
+      <c r="R7" s="2">
+        <v>0</v>
+      </c>
+      <c r="S7" s="2">
+        <v>0</v>
+      </c>
+      <c r="T7" s="2">
+        <v>0</v>
+      </c>
+      <c r="U7" s="2">
+        <v>0</v>
+      </c>
+      <c r="V7" s="2">
+        <v>0</v>
+      </c>
+      <c r="W7" s="2">
+        <v>0</v>
+      </c>
+      <c r="X7" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y7" s="2">
+        <v>11</v>
+      </c>
+      <c r="Z7" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA7" s="2">
+        <v>1</v>
+      </c>
+      <c r="AB7" s="2">
+        <v>1</v>
+      </c>
+      <c r="AC7" s="2">
+        <v>1</v>
+      </c>
+      <c r="AD7" s="2">
+        <v>8</v>
+      </c>
+      <c r="AE7" s="2">
+        <v>1</v>
+      </c>
+      <c r="AF7" s="2">
+        <v>0</v>
+      </c>
+      <c r="AG7" s="2">
+        <v>0</v>
+      </c>
+      <c r="AH7" s="2">
+        <v>1</v>
+      </c>
+      <c r="AI7" s="2">
+        <v>0</v>
+      </c>
+      <c r="AJ7" s="2">
+        <v>0</v>
+      </c>
+      <c r="AK7" s="2">
+        <v>1</v>
+      </c>
+      <c r="AL7" s="2">
+        <v>0</v>
+      </c>
+      <c r="AM7" s="2">
         <v>2</v>
       </c>
-      <c r="E7" s="2">
-        <v>0</v>
-      </c>
-      <c r="F7" s="2">
-        <v>1</v>
-      </c>
-      <c r="G7" s="2">
-        <v>0</v>
-      </c>
-      <c r="H7" s="2">
-        <v>0</v>
-      </c>
-      <c r="I7" s="2">
-        <v>1</v>
-      </c>
-      <c r="J7" s="2">
-        <v>0</v>
-      </c>
-      <c r="K7" s="2">
-        <v>0</v>
-      </c>
-      <c r="L7" s="2">
-        <v>1</v>
-      </c>
-      <c r="M7" s="2">
-        <v>8</v>
-      </c>
-      <c r="N7" s="2">
-        <v>1</v>
-      </c>
-      <c r="O7" s="2">
-        <v>1</v>
-      </c>
-      <c r="P7" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q7" s="2">
-        <v>1</v>
-      </c>
-      <c r="R7" s="2">
-        <v>11</v>
-      </c>
-      <c r="S7" s="2">
-        <v>0</v>
-      </c>
-      <c r="T7" s="2">
-        <v>0</v>
-      </c>
-      <c r="U7" s="2">
-        <v>0</v>
-      </c>
-      <c r="V7" s="2">
-        <v>0</v>
-      </c>
-      <c r="W7" s="2">
-        <v>0</v>
-      </c>
-      <c r="X7" s="2">
-        <v>0</v>
-      </c>
-      <c r="Y7" s="2">
-        <v>0</v>
-      </c>
-      <c r="Z7" s="2">
-        <v>0</v>
-      </c>
-      <c r="AA7" s="2">
-        <v>1</v>
-      </c>
-      <c r="AB7" s="2">
-        <v>0</v>
-      </c>
-      <c r="AC7" s="2">
-        <v>1</v>
-      </c>
-      <c r="AD7" s="2">
-        <v>0</v>
-      </c>
-      <c r="AE7" s="2">
-        <v>1</v>
-      </c>
-      <c r="AF7" s="2">
-        <v>0</v>
-      </c>
-      <c r="AG7" s="2">
-        <v>1</v>
-      </c>
-      <c r="AH7" s="2">
-        <v>1</v>
-      </c>
-      <c r="AI7" s="2">
-        <v>1</v>
-      </c>
-      <c r="AJ7" s="2">
-        <v>0</v>
-      </c>
-      <c r="AK7" s="2">
-        <v>0</v>
-      </c>
-      <c r="AL7" s="2">
-        <v>0</v>
-      </c>
-      <c r="AM7" s="2">
-        <v>0</v>
-      </c>
       <c r="AN7" s="2">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="AO7" s="2">
         <v>0</v>
@@ -1528,22 +1528,22 @@
         <v>2</v>
       </c>
       <c r="C8" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D8" s="2">
         <v>0</v>
       </c>
       <c r="E8" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F8" s="2">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="G8" s="2">
         <v>0</v>
       </c>
       <c r="H8" s="2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I8" s="2">
         <v>0</v>
@@ -1558,59 +1558,59 @@
         <v>0</v>
       </c>
       <c r="M8" s="2">
+        <v>0</v>
+      </c>
+      <c r="N8" s="2">
+        <v>2</v>
+      </c>
+      <c r="O8" s="2">
+        <v>1</v>
+      </c>
+      <c r="P8" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="2">
+        <v>0</v>
+      </c>
+      <c r="R8" s="2">
+        <v>0</v>
+      </c>
+      <c r="S8" s="2">
+        <v>1</v>
+      </c>
+      <c r="T8" s="2">
+        <v>0</v>
+      </c>
+      <c r="U8" s="2">
+        <v>0</v>
+      </c>
+      <c r="V8" s="2">
+        <v>1</v>
+      </c>
+      <c r="W8" s="2">
+        <v>0</v>
+      </c>
+      <c r="X8" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y8" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z8" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA8" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB8" s="2">
+        <v>1</v>
+      </c>
+      <c r="AC8" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD8" s="2">
         <v>6</v>
       </c>
-      <c r="N8" s="2">
-        <v>0</v>
-      </c>
-      <c r="O8" s="2">
-        <v>1</v>
-      </c>
-      <c r="P8" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q8" s="2">
-        <v>0</v>
-      </c>
-      <c r="R8" s="2">
-        <v>1</v>
-      </c>
-      <c r="S8" s="2">
-        <v>0</v>
-      </c>
-      <c r="T8" s="2">
-        <v>0</v>
-      </c>
-      <c r="U8" s="2">
-        <v>1</v>
-      </c>
-      <c r="V8" s="2">
-        <v>0</v>
-      </c>
-      <c r="W8" s="2">
-        <v>0</v>
-      </c>
-      <c r="X8" s="2">
-        <v>1</v>
-      </c>
-      <c r="Y8" s="2">
-        <v>0</v>
-      </c>
-      <c r="Z8" s="2">
-        <v>0</v>
-      </c>
-      <c r="AA8" s="2">
-        <v>0</v>
-      </c>
-      <c r="AB8" s="2">
-        <v>1</v>
-      </c>
-      <c r="AC8" s="2">
-        <v>2</v>
-      </c>
-      <c r="AD8" s="2">
-        <v>0</v>
-      </c>
       <c r="AE8" s="2">
         <v>0</v>
       </c>
@@ -1624,22 +1624,22 @@
         <v>0</v>
       </c>
       <c r="AI8" s="2">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AJ8" s="2">
         <v>0</v>
       </c>
       <c r="AK8" s="2">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="AL8" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM8" s="2">
         <v>0</v>
       </c>
       <c r="AN8" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AO8" s="2">
         <v>2</v>
@@ -1653,124 +1653,124 @@
         <v>48</v>
       </c>
       <c r="B9" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C9" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D9" s="2">
+        <v>1</v>
+      </c>
+      <c r="E9" s="2">
+        <v>0</v>
+      </c>
+      <c r="F9" s="2">
+        <v>1</v>
+      </c>
+      <c r="G9" s="2">
+        <v>0</v>
+      </c>
+      <c r="H9" s="2">
+        <v>0</v>
+      </c>
+      <c r="I9" s="2">
+        <v>1</v>
+      </c>
+      <c r="J9" s="2">
+        <v>0</v>
+      </c>
+      <c r="K9" s="2">
+        <v>0</v>
+      </c>
+      <c r="L9" s="2">
+        <v>1</v>
+      </c>
+      <c r="M9" s="2">
+        <v>0</v>
+      </c>
+      <c r="N9" s="2">
+        <v>0</v>
+      </c>
+      <c r="O9" s="2">
+        <v>0</v>
+      </c>
+      <c r="P9" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q9" s="2">
+        <v>0</v>
+      </c>
+      <c r="R9" s="2">
+        <v>0</v>
+      </c>
+      <c r="S9" s="2">
+        <v>0</v>
+      </c>
+      <c r="T9" s="2">
+        <v>1</v>
+      </c>
+      <c r="U9" s="2">
+        <v>0</v>
+      </c>
+      <c r="V9" s="2">
+        <v>1</v>
+      </c>
+      <c r="W9" s="2">
+        <v>1</v>
+      </c>
+      <c r="X9" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y9" s="2">
         <v>2</v>
       </c>
-      <c r="E9" s="2">
-        <v>0</v>
-      </c>
-      <c r="F9" s="2">
+      <c r="Z9" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA9" s="2">
+        <v>3</v>
+      </c>
+      <c r="AB9" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC9" s="2">
+        <v>10</v>
+      </c>
+      <c r="AD9" s="2">
+        <v>1</v>
+      </c>
+      <c r="AE9" s="2">
+        <v>0</v>
+      </c>
+      <c r="AF9" s="2">
+        <v>0</v>
+      </c>
+      <c r="AG9" s="2">
+        <v>0</v>
+      </c>
+      <c r="AH9" s="2">
+        <v>0</v>
+      </c>
+      <c r="AI9" s="2">
+        <v>0</v>
+      </c>
+      <c r="AJ9" s="2">
+        <v>0</v>
+      </c>
+      <c r="AK9" s="2">
         <v>2</v>
       </c>
-      <c r="G9" s="2">
-        <v>0</v>
-      </c>
-      <c r="H9" s="2">
-        <v>0</v>
-      </c>
-      <c r="I9" s="2">
-        <v>0</v>
-      </c>
-      <c r="J9" s="2">
-        <v>0</v>
-      </c>
-      <c r="K9" s="2">
-        <v>0</v>
-      </c>
-      <c r="L9" s="2">
-        <v>0</v>
-      </c>
-      <c r="M9" s="2">
-        <v>1</v>
-      </c>
-      <c r="N9" s="2">
-        <v>10</v>
-      </c>
-      <c r="O9" s="2">
-        <v>0</v>
-      </c>
-      <c r="P9" s="2">
-        <v>3</v>
-      </c>
-      <c r="Q9" s="2">
-        <v>0</v>
-      </c>
-      <c r="R9" s="2">
+      <c r="AL9" s="2">
+        <v>0</v>
+      </c>
+      <c r="AM9" s="2">
         <v>2</v>
       </c>
-      <c r="S9" s="2">
-        <v>0</v>
-      </c>
-      <c r="T9" s="2">
-        <v>1</v>
-      </c>
-      <c r="U9" s="2">
-        <v>1</v>
-      </c>
-      <c r="V9" s="2">
-        <v>0</v>
-      </c>
-      <c r="W9" s="2">
-        <v>1</v>
-      </c>
-      <c r="X9" s="2">
-        <v>0</v>
-      </c>
-      <c r="Y9" s="2">
-        <v>0</v>
-      </c>
-      <c r="Z9" s="2">
-        <v>0</v>
-      </c>
-      <c r="AA9" s="2">
-        <v>1</v>
-      </c>
-      <c r="AB9" s="2">
-        <v>0</v>
-      </c>
-      <c r="AC9" s="2">
-        <v>0</v>
-      </c>
-      <c r="AD9" s="2">
-        <v>0</v>
-      </c>
-      <c r="AE9" s="2">
-        <v>1</v>
-      </c>
-      <c r="AF9" s="2">
-        <v>0</v>
-      </c>
-      <c r="AG9" s="2">
-        <v>0</v>
-      </c>
-      <c r="AH9" s="2">
-        <v>1</v>
-      </c>
-      <c r="AI9" s="2">
-        <v>0</v>
-      </c>
-      <c r="AJ9" s="2">
-        <v>0</v>
-      </c>
-      <c r="AK9" s="2">
-        <v>1</v>
-      </c>
-      <c r="AL9" s="2">
-        <v>0</v>
-      </c>
-      <c r="AM9" s="2">
-        <v>1</v>
-      </c>
       <c r="AN9" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AO9" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AP9" s="2">
         <v>31</v>
@@ -1781,25 +1781,25 @@
         <v>49</v>
       </c>
       <c r="B10" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C10" s="2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D10" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E10" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F10" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G10" s="2">
         <v>0</v>
       </c>
       <c r="H10" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I10" s="2">
         <v>0</v>
@@ -1817,53 +1817,53 @@
         <v>0</v>
       </c>
       <c r="N10" s="2">
+        <v>0</v>
+      </c>
+      <c r="O10" s="2">
+        <v>0</v>
+      </c>
+      <c r="P10" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q10" s="2">
+        <v>0</v>
+      </c>
+      <c r="R10" s="2">
+        <v>0</v>
+      </c>
+      <c r="S10" s="2">
+        <v>0</v>
+      </c>
+      <c r="T10" s="2">
+        <v>0</v>
+      </c>
+      <c r="U10" s="2">
         <v>2</v>
       </c>
-      <c r="O10" s="2">
-        <v>1</v>
-      </c>
-      <c r="P10" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q10" s="2">
-        <v>0</v>
-      </c>
-      <c r="R10" s="2">
-        <v>0</v>
-      </c>
-      <c r="S10" s="2">
-        <v>0</v>
-      </c>
-      <c r="T10" s="2">
-        <v>0</v>
-      </c>
-      <c r="U10" s="2">
-        <v>0</v>
-      </c>
       <c r="V10" s="2">
+        <v>0</v>
+      </c>
+      <c r="W10" s="2">
+        <v>0</v>
+      </c>
+      <c r="X10" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y10" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z10" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA10" s="2">
+        <v>1</v>
+      </c>
+      <c r="AB10" s="2">
+        <v>1</v>
+      </c>
+      <c r="AC10" s="2">
         <v>2</v>
       </c>
-      <c r="W10" s="2">
-        <v>0</v>
-      </c>
-      <c r="X10" s="2">
-        <v>0</v>
-      </c>
-      <c r="Y10" s="2">
-        <v>0</v>
-      </c>
-      <c r="Z10" s="2">
-        <v>0</v>
-      </c>
-      <c r="AA10" s="2">
-        <v>1</v>
-      </c>
-      <c r="AB10" s="2">
-        <v>0</v>
-      </c>
-      <c r="AC10" s="2">
-        <v>0</v>
-      </c>
       <c r="AD10" s="2">
         <v>0</v>
       </c>
@@ -1880,25 +1880,25 @@
         <v>0</v>
       </c>
       <c r="AI10" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AJ10" s="2">
         <v>0</v>
       </c>
       <c r="AK10" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL10" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM10" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AN10" s="2">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AO10" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AP10" s="2">
         <v>22</v>
@@ -1909,19 +1909,19 @@
         <v>50</v>
       </c>
       <c r="B11" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C11" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D11" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E11" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F11" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G11" s="2">
         <v>0</v>
@@ -1939,64 +1939,64 @@
         <v>0</v>
       </c>
       <c r="L11" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M11" s="2">
+        <v>0</v>
+      </c>
+      <c r="N11" s="2">
+        <v>1</v>
+      </c>
+      <c r="O11" s="2">
+        <v>0</v>
+      </c>
+      <c r="P11" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q11" s="2">
+        <v>0</v>
+      </c>
+      <c r="R11" s="2">
+        <v>0</v>
+      </c>
+      <c r="S11" s="2">
+        <v>0</v>
+      </c>
+      <c r="T11" s="2">
+        <v>6</v>
+      </c>
+      <c r="U11" s="2">
+        <v>0</v>
+      </c>
+      <c r="V11" s="2">
+        <v>0</v>
+      </c>
+      <c r="W11" s="2">
+        <v>0</v>
+      </c>
+      <c r="X11" s="2">
+        <v>1</v>
+      </c>
+      <c r="Y11" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z11" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA11" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB11" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC11" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD11" s="2">
         <v>5</v>
       </c>
-      <c r="N11" s="2">
-        <v>0</v>
-      </c>
-      <c r="O11" s="2">
-        <v>0</v>
-      </c>
-      <c r="P11" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q11" s="2">
-        <v>0</v>
-      </c>
-      <c r="R11" s="2">
-        <v>0</v>
-      </c>
-      <c r="S11" s="2">
-        <v>1</v>
-      </c>
-      <c r="T11" s="2">
-        <v>0</v>
-      </c>
-      <c r="U11" s="2">
-        <v>0</v>
-      </c>
-      <c r="V11" s="2">
-        <v>0</v>
-      </c>
-      <c r="W11" s="2">
-        <v>6</v>
-      </c>
-      <c r="X11" s="2">
-        <v>0</v>
-      </c>
-      <c r="Y11" s="2">
-        <v>0</v>
-      </c>
-      <c r="Z11" s="2">
-        <v>0</v>
-      </c>
-      <c r="AA11" s="2">
-        <v>1</v>
-      </c>
-      <c r="AB11" s="2">
-        <v>0</v>
-      </c>
-      <c r="AC11" s="2">
-        <v>1</v>
-      </c>
-      <c r="AD11" s="2">
-        <v>0</v>
-      </c>
       <c r="AE11" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF11" s="2">
         <v>0</v>
@@ -2014,19 +2014,19 @@
         <v>0</v>
       </c>
       <c r="AK11" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL11" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM11" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN11" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AO11" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AP11" s="2">
         <v>21</v>
@@ -2043,7 +2043,7 @@
         <v>1</v>
       </c>
       <c r="D12" s="2">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E12" s="2">
         <v>0</v>
@@ -2055,7 +2055,7 @@
         <v>0</v>
       </c>
       <c r="H12" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I12" s="2">
         <v>0</v>
@@ -2064,7 +2064,7 @@
         <v>0</v>
       </c>
       <c r="K12" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L12" s="2">
         <v>0</v>
@@ -2073,7 +2073,7 @@
         <v>0</v>
       </c>
       <c r="N12" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O12" s="2">
         <v>0</v>
@@ -2094,10 +2094,10 @@
         <v>0</v>
       </c>
       <c r="U12" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V12" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W12" s="2">
         <v>0</v>
@@ -2118,7 +2118,7 @@
         <v>0</v>
       </c>
       <c r="AC12" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD12" s="2">
         <v>0</v>
@@ -2127,7 +2127,7 @@
         <v>0</v>
       </c>
       <c r="AF12" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG12" s="2">
         <v>0</v>
@@ -2136,7 +2136,7 @@
         <v>0</v>
       </c>
       <c r="AI12" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ12" s="2">
         <v>0</v>
@@ -2148,7 +2148,7 @@
         <v>0</v>
       </c>
       <c r="AM12" s="2">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="AN12" s="2">
         <v>1</v>
@@ -2168,7 +2168,7 @@
         <v>0</v>
       </c>
       <c r="C13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D13" s="2">
         <v>0</v>
@@ -2201,53 +2201,53 @@
         <v>0</v>
       </c>
       <c r="N13" s="2">
+        <v>0</v>
+      </c>
+      <c r="O13" s="2">
+        <v>0</v>
+      </c>
+      <c r="P13" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="2">
+        <v>0</v>
+      </c>
+      <c r="R13" s="2">
+        <v>0</v>
+      </c>
+      <c r="S13" s="2">
+        <v>0</v>
+      </c>
+      <c r="T13" s="2">
+        <v>0</v>
+      </c>
+      <c r="U13" s="2">
+        <v>0</v>
+      </c>
+      <c r="V13" s="2">
+        <v>0</v>
+      </c>
+      <c r="W13" s="2">
+        <v>1</v>
+      </c>
+      <c r="X13" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y13" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z13" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA13" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB13" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC13" s="2">
         <v>13</v>
       </c>
-      <c r="O13" s="2">
-        <v>0</v>
-      </c>
-      <c r="P13" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q13" s="2">
-        <v>0</v>
-      </c>
-      <c r="R13" s="2">
-        <v>0</v>
-      </c>
-      <c r="S13" s="2">
-        <v>0</v>
-      </c>
-      <c r="T13" s="2">
-        <v>1</v>
-      </c>
-      <c r="U13" s="2">
-        <v>0</v>
-      </c>
-      <c r="V13" s="2">
-        <v>0</v>
-      </c>
-      <c r="W13" s="2">
-        <v>0</v>
-      </c>
-      <c r="X13" s="2">
-        <v>0</v>
-      </c>
-      <c r="Y13" s="2">
-        <v>0</v>
-      </c>
-      <c r="Z13" s="2">
-        <v>0</v>
-      </c>
-      <c r="AA13" s="2">
-        <v>0</v>
-      </c>
-      <c r="AB13" s="2">
-        <v>0</v>
-      </c>
-      <c r="AC13" s="2">
-        <v>0</v>
-      </c>
       <c r="AD13" s="2">
         <v>0</v>
       </c>
@@ -2279,7 +2279,7 @@
         <v>0</v>
       </c>
       <c r="AN13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AO13" s="2">
         <v>0</v>
@@ -2293,13 +2293,13 @@
         <v>53</v>
       </c>
       <c r="B14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D14" s="2">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E14" s="2">
         <v>0</v>
@@ -2311,7 +2311,7 @@
         <v>0</v>
       </c>
       <c r="H14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I14" s="2">
         <v>0</v>
@@ -2350,10 +2350,10 @@
         <v>0</v>
       </c>
       <c r="U14" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V14" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="W14" s="2">
         <v>0</v>
@@ -2392,7 +2392,7 @@
         <v>0</v>
       </c>
       <c r="AI14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ14" s="2">
         <v>0</v>
@@ -2404,13 +2404,13 @@
         <v>0</v>
       </c>
       <c r="AM14" s="2">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="AN14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AO14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AP14" s="2">
         <v>11</v>
@@ -2424,19 +2424,19 @@
         <v>1</v>
       </c>
       <c r="C15" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D15" s="2">
         <v>0</v>
       </c>
       <c r="E15" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F15" s="2">
         <v>0</v>
       </c>
       <c r="G15" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H15" s="2">
         <v>0</v>
@@ -2451,7 +2451,7 @@
         <v>0</v>
       </c>
       <c r="L15" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M15" s="2">
         <v>0</v>
@@ -2469,7 +2469,7 @@
         <v>0</v>
       </c>
       <c r="R15" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="S15" s="2">
         <v>0</v>
@@ -2490,7 +2490,7 @@
         <v>0</v>
       </c>
       <c r="Y15" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Z15" s="2">
         <v>0</v>
@@ -2508,7 +2508,7 @@
         <v>0</v>
       </c>
       <c r="AE15" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AF15" s="2">
         <v>0</v>
@@ -2523,19 +2523,19 @@
         <v>0</v>
       </c>
       <c r="AJ15" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK15" s="2">
         <v>0</v>
       </c>
       <c r="AL15" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM15" s="2">
         <v>0</v>
       </c>
       <c r="AN15" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AO15" s="2">
         <v>1</v>
@@ -2552,7 +2552,7 @@
         <v>0</v>
       </c>
       <c r="C16" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D16" s="2">
         <v>0</v>
@@ -2567,10 +2567,10 @@
         <v>0</v>
       </c>
       <c r="H16" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I16" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J16" s="2">
         <v>0</v>
@@ -2597,29 +2597,29 @@
         <v>0</v>
       </c>
       <c r="R16" s="2">
+        <v>1</v>
+      </c>
+      <c r="S16" s="2">
+        <v>0</v>
+      </c>
+      <c r="T16" s="2">
+        <v>0</v>
+      </c>
+      <c r="U16" s="2">
+        <v>0</v>
+      </c>
+      <c r="V16" s="2">
+        <v>0</v>
+      </c>
+      <c r="W16" s="2">
+        <v>0</v>
+      </c>
+      <c r="X16" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y16" s="2">
         <v>2</v>
       </c>
-      <c r="S16" s="2">
-        <v>0</v>
-      </c>
-      <c r="T16" s="2">
-        <v>0</v>
-      </c>
-      <c r="U16" s="2">
-        <v>0</v>
-      </c>
-      <c r="V16" s="2">
-        <v>0</v>
-      </c>
-      <c r="W16" s="2">
-        <v>0</v>
-      </c>
-      <c r="X16" s="2">
-        <v>0</v>
-      </c>
-      <c r="Y16" s="2">
-        <v>1</v>
-      </c>
       <c r="Z16" s="2">
         <v>0</v>
       </c>
@@ -2645,10 +2645,10 @@
         <v>0</v>
       </c>
       <c r="AH16" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI16" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ16" s="2">
         <v>0</v>
@@ -2663,7 +2663,7 @@
         <v>0</v>
       </c>
       <c r="AN16" s="2">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="AO16" s="2">
         <v>0</v>
@@ -2677,10 +2677,10 @@
         <v>56</v>
       </c>
       <c r="B17" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C17" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D17" s="2">
         <v>1</v>
@@ -2689,13 +2689,13 @@
         <v>0</v>
       </c>
       <c r="F17" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G17" s="2">
         <v>0</v>
       </c>
       <c r="H17" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I17" s="2">
         <v>0</v>
@@ -2713,52 +2713,52 @@
         <v>0</v>
       </c>
       <c r="N17" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O17" s="2">
+        <v>0</v>
+      </c>
+      <c r="P17" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="2">
+        <v>0</v>
+      </c>
+      <c r="R17" s="2">
+        <v>0</v>
+      </c>
+      <c r="S17" s="2">
+        <v>0</v>
+      </c>
+      <c r="T17" s="2">
+        <v>0</v>
+      </c>
+      <c r="U17" s="2">
+        <v>0</v>
+      </c>
+      <c r="V17" s="2">
+        <v>0</v>
+      </c>
+      <c r="W17" s="2">
+        <v>0</v>
+      </c>
+      <c r="X17" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y17" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z17" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA17" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB17" s="2">
         <v>2</v>
       </c>
-      <c r="P17" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q17" s="2">
-        <v>0</v>
-      </c>
-      <c r="R17" s="2">
-        <v>0</v>
-      </c>
-      <c r="S17" s="2">
-        <v>0</v>
-      </c>
-      <c r="T17" s="2">
-        <v>0</v>
-      </c>
-      <c r="U17" s="2">
-        <v>0</v>
-      </c>
-      <c r="V17" s="2">
-        <v>0</v>
-      </c>
-      <c r="W17" s="2">
-        <v>0</v>
-      </c>
-      <c r="X17" s="2">
-        <v>0</v>
-      </c>
-      <c r="Y17" s="2">
-        <v>0</v>
-      </c>
-      <c r="Z17" s="2">
-        <v>0</v>
-      </c>
-      <c r="AA17" s="2">
-        <v>0</v>
-      </c>
-      <c r="AB17" s="2">
-        <v>0</v>
-      </c>
       <c r="AC17" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD17" s="2">
         <v>0</v>
@@ -2776,13 +2776,13 @@
         <v>0</v>
       </c>
       <c r="AI17" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ17" s="2">
         <v>0</v>
       </c>
       <c r="AK17" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL17" s="2">
         <v>0</v>
@@ -2791,10 +2791,10 @@
         <v>1</v>
       </c>
       <c r="AN17" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AO17" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AP17" s="2">
         <v>9</v>
@@ -2805,19 +2805,19 @@
         <v>57</v>
       </c>
       <c r="B18" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C18" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D18" s="2">
         <v>0</v>
       </c>
       <c r="E18" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F18" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G18" s="2">
         <v>0</v>
@@ -2835,25 +2835,25 @@
         <v>0</v>
       </c>
       <c r="L18" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M18" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N18" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O18" s="2">
         <v>0</v>
       </c>
       <c r="P18" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q18" s="2">
         <v>0</v>
       </c>
       <c r="R18" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S18" s="2">
         <v>0</v>
@@ -2874,25 +2874,25 @@
         <v>0</v>
       </c>
       <c r="Y18" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z18" s="2">
         <v>0</v>
       </c>
       <c r="AA18" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB18" s="2">
         <v>0</v>
       </c>
       <c r="AC18" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD18" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE18" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF18" s="2">
         <v>0</v>
@@ -2910,19 +2910,19 @@
         <v>0</v>
       </c>
       <c r="AK18" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL18" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM18" s="2">
         <v>0</v>
       </c>
       <c r="AN18" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AO18" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AP18" s="2">
         <v>9</v>
@@ -2936,7 +2936,7 @@
         <v>0</v>
       </c>
       <c r="C19" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D19" s="2">
         <v>0</v>
@@ -2969,53 +2969,53 @@
         <v>0</v>
       </c>
       <c r="N19" s="2">
+        <v>0</v>
+      </c>
+      <c r="O19" s="2">
+        <v>0</v>
+      </c>
+      <c r="P19" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q19" s="2">
+        <v>0</v>
+      </c>
+      <c r="R19" s="2">
+        <v>0</v>
+      </c>
+      <c r="S19" s="2">
+        <v>0</v>
+      </c>
+      <c r="T19" s="2">
+        <v>0</v>
+      </c>
+      <c r="U19" s="2">
+        <v>0</v>
+      </c>
+      <c r="V19" s="2">
+        <v>0</v>
+      </c>
+      <c r="W19" s="2">
+        <v>0</v>
+      </c>
+      <c r="X19" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y19" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z19" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA19" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB19" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC19" s="2">
         <v>6</v>
       </c>
-      <c r="O19" s="2">
-        <v>0</v>
-      </c>
-      <c r="P19" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q19" s="2">
-        <v>0</v>
-      </c>
-      <c r="R19" s="2">
-        <v>0</v>
-      </c>
-      <c r="S19" s="2">
-        <v>0</v>
-      </c>
-      <c r="T19" s="2">
-        <v>0</v>
-      </c>
-      <c r="U19" s="2">
-        <v>0</v>
-      </c>
-      <c r="V19" s="2">
-        <v>0</v>
-      </c>
-      <c r="W19" s="2">
-        <v>0</v>
-      </c>
-      <c r="X19" s="2">
-        <v>0</v>
-      </c>
-      <c r="Y19" s="2">
-        <v>0</v>
-      </c>
-      <c r="Z19" s="2">
-        <v>0</v>
-      </c>
-      <c r="AA19" s="2">
-        <v>0</v>
-      </c>
-      <c r="AB19" s="2">
-        <v>0</v>
-      </c>
-      <c r="AC19" s="2">
-        <v>0</v>
-      </c>
       <c r="AD19" s="2">
         <v>0</v>
       </c>
@@ -3047,7 +3047,7 @@
         <v>0</v>
       </c>
       <c r="AN19" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AO19" s="2">
         <v>0</v>
@@ -3073,13 +3073,13 @@
         <v>0</v>
       </c>
       <c r="F20" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G20" s="2">
         <v>0</v>
       </c>
       <c r="H20" s="2">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="I20" s="2">
         <v>0</v>
@@ -3100,7 +3100,7 @@
         <v>0</v>
       </c>
       <c r="O20" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P20" s="2">
         <v>0</v>
@@ -3139,7 +3139,7 @@
         <v>0</v>
       </c>
       <c r="AB20" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC20" s="2">
         <v>0</v>
@@ -3160,13 +3160,13 @@
         <v>0</v>
       </c>
       <c r="AI20" s="2">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="AJ20" s="2">
         <v>0</v>
       </c>
       <c r="AK20" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL20" s="2">
         <v>0</v>
@@ -3189,10 +3189,10 @@
         <v>60</v>
       </c>
       <c r="B21" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C21" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D21" s="2">
         <v>0</v>
@@ -3207,7 +3207,7 @@
         <v>0</v>
       </c>
       <c r="H21" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I21" s="2">
         <v>0</v>
@@ -3219,7 +3219,7 @@
         <v>0</v>
       </c>
       <c r="L21" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M21" s="2">
         <v>0</v>
@@ -3228,7 +3228,7 @@
         <v>0</v>
       </c>
       <c r="O21" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P21" s="2">
         <v>0</v>
@@ -3237,7 +3237,7 @@
         <v>0</v>
       </c>
       <c r="R21" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S21" s="2">
         <v>0</v>
@@ -3258,7 +3258,7 @@
         <v>0</v>
       </c>
       <c r="Y21" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z21" s="2">
         <v>0</v>
@@ -3267,7 +3267,7 @@
         <v>0</v>
       </c>
       <c r="AB21" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC21" s="2">
         <v>0</v>
@@ -3276,7 +3276,7 @@
         <v>0</v>
       </c>
       <c r="AE21" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF21" s="2">
         <v>0</v>
@@ -3288,7 +3288,7 @@
         <v>0</v>
       </c>
       <c r="AI21" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AJ21" s="2">
         <v>0</v>
@@ -3303,10 +3303,10 @@
         <v>0</v>
       </c>
       <c r="AN21" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AO21" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AP21" s="2">
         <v>7</v>
@@ -3317,124 +3317,124 @@
         <v>61</v>
       </c>
       <c r="B22" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C22" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D22" s="2">
+        <v>0</v>
+      </c>
+      <c r="E22" s="2">
+        <v>0</v>
+      </c>
+      <c r="F22" s="2">
+        <v>0</v>
+      </c>
+      <c r="G22" s="2">
+        <v>0</v>
+      </c>
+      <c r="H22" s="2">
+        <v>0</v>
+      </c>
+      <c r="I22" s="2">
+        <v>0</v>
+      </c>
+      <c r="J22" s="2">
+        <v>0</v>
+      </c>
+      <c r="K22" s="2">
+        <v>0</v>
+      </c>
+      <c r="L22" s="2">
+        <v>0</v>
+      </c>
+      <c r="M22" s="2">
+        <v>0</v>
+      </c>
+      <c r="N22" s="2">
+        <v>1</v>
+      </c>
+      <c r="O22" s="2">
+        <v>0</v>
+      </c>
+      <c r="P22" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q22" s="2">
+        <v>0</v>
+      </c>
+      <c r="R22" s="2">
+        <v>0</v>
+      </c>
+      <c r="S22" s="2">
+        <v>0</v>
+      </c>
+      <c r="T22" s="2">
+        <v>0</v>
+      </c>
+      <c r="U22" s="2">
+        <v>0</v>
+      </c>
+      <c r="V22" s="2">
+        <v>0</v>
+      </c>
+      <c r="W22" s="2">
+        <v>0</v>
+      </c>
+      <c r="X22" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y22" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z22" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA22" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB22" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC22" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD22" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE22" s="2">
+        <v>0</v>
+      </c>
+      <c r="AF22" s="2">
+        <v>0</v>
+      </c>
+      <c r="AG22" s="2">
+        <v>0</v>
+      </c>
+      <c r="AH22" s="2">
+        <v>0</v>
+      </c>
+      <c r="AI22" s="2">
+        <v>0</v>
+      </c>
+      <c r="AJ22" s="2">
+        <v>0</v>
+      </c>
+      <c r="AK22" s="2">
+        <v>0</v>
+      </c>
+      <c r="AL22" s="2">
+        <v>1</v>
+      </c>
+      <c r="AM22" s="2">
         <v>2</v>
       </c>
-      <c r="E22" s="2">
-        <v>1</v>
-      </c>
-      <c r="F22" s="2">
-        <v>0</v>
-      </c>
-      <c r="G22" s="2">
-        <v>0</v>
-      </c>
-      <c r="H22" s="2">
-        <v>0</v>
-      </c>
-      <c r="I22" s="2">
-        <v>0</v>
-      </c>
-      <c r="J22" s="2">
-        <v>0</v>
-      </c>
-      <c r="K22" s="2">
-        <v>0</v>
-      </c>
-      <c r="L22" s="2">
-        <v>0</v>
-      </c>
-      <c r="M22" s="2">
-        <v>0</v>
-      </c>
-      <c r="N22" s="2">
-        <v>0</v>
-      </c>
-      <c r="O22" s="2">
-        <v>0</v>
-      </c>
-      <c r="P22" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q22" s="2">
-        <v>0</v>
-      </c>
-      <c r="R22" s="2">
-        <v>0</v>
-      </c>
-      <c r="S22" s="2">
-        <v>0</v>
-      </c>
-      <c r="T22" s="2">
-        <v>0</v>
-      </c>
-      <c r="U22" s="2">
-        <v>0</v>
-      </c>
-      <c r="V22" s="2">
-        <v>0</v>
-      </c>
-      <c r="W22" s="2">
-        <v>0</v>
-      </c>
-      <c r="X22" s="2">
-        <v>0</v>
-      </c>
-      <c r="Y22" s="2">
-        <v>0</v>
-      </c>
-      <c r="Z22" s="2">
-        <v>0</v>
-      </c>
-      <c r="AA22" s="2">
-        <v>0</v>
-      </c>
-      <c r="AB22" s="2">
-        <v>0</v>
-      </c>
-      <c r="AC22" s="2">
-        <v>1</v>
-      </c>
-      <c r="AD22" s="2">
-        <v>0</v>
-      </c>
-      <c r="AE22" s="2">
-        <v>0</v>
-      </c>
-      <c r="AF22" s="2">
-        <v>0</v>
-      </c>
-      <c r="AG22" s="2">
-        <v>0</v>
-      </c>
-      <c r="AH22" s="2">
-        <v>0</v>
-      </c>
-      <c r="AI22" s="2">
-        <v>0</v>
-      </c>
-      <c r="AJ22" s="2">
-        <v>0</v>
-      </c>
-      <c r="AK22" s="2">
-        <v>0</v>
-      </c>
-      <c r="AL22" s="2">
-        <v>0</v>
-      </c>
-      <c r="AM22" s="2">
-        <v>0</v>
-      </c>
       <c r="AN22" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AO22" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AP22" s="2">
         <v>7</v>
@@ -3448,118 +3448,118 @@
         <v>0</v>
       </c>
       <c r="C23" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D23" s="2">
         <v>0</v>
       </c>
       <c r="E23" s="2">
+        <v>0</v>
+      </c>
+      <c r="F23" s="2">
+        <v>0</v>
+      </c>
+      <c r="G23" s="2">
+        <v>0</v>
+      </c>
+      <c r="H23" s="2">
+        <v>0</v>
+      </c>
+      <c r="I23" s="2">
+        <v>0</v>
+      </c>
+      <c r="J23" s="2">
+        <v>0</v>
+      </c>
+      <c r="K23" s="2">
+        <v>0</v>
+      </c>
+      <c r="L23" s="2">
+        <v>1</v>
+      </c>
+      <c r="M23" s="2">
+        <v>0</v>
+      </c>
+      <c r="N23" s="2">
+        <v>0</v>
+      </c>
+      <c r="O23" s="2">
+        <v>0</v>
+      </c>
+      <c r="P23" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q23" s="2">
+        <v>0</v>
+      </c>
+      <c r="R23" s="2">
+        <v>0</v>
+      </c>
+      <c r="S23" s="2">
+        <v>0</v>
+      </c>
+      <c r="T23" s="2">
+        <v>0</v>
+      </c>
+      <c r="U23" s="2">
+        <v>0</v>
+      </c>
+      <c r="V23" s="2">
+        <v>0</v>
+      </c>
+      <c r="W23" s="2">
+        <v>0</v>
+      </c>
+      <c r="X23" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y23" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z23" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA23" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB23" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC23" s="2">
+        <v>1</v>
+      </c>
+      <c r="AD23" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE23" s="2">
+        <v>0</v>
+      </c>
+      <c r="AF23" s="2">
+        <v>0</v>
+      </c>
+      <c r="AG23" s="2">
+        <v>0</v>
+      </c>
+      <c r="AH23" s="2">
+        <v>0</v>
+      </c>
+      <c r="AI23" s="2">
+        <v>0</v>
+      </c>
+      <c r="AJ23" s="2">
+        <v>0</v>
+      </c>
+      <c r="AK23" s="2">
+        <v>0</v>
+      </c>
+      <c r="AL23" s="2">
         <v>3</v>
       </c>
-      <c r="F23" s="2">
-        <v>0</v>
-      </c>
-      <c r="G23" s="2">
-        <v>0</v>
-      </c>
-      <c r="H23" s="2">
-        <v>0</v>
-      </c>
-      <c r="I23" s="2">
-        <v>0</v>
-      </c>
-      <c r="J23" s="2">
-        <v>0</v>
-      </c>
-      <c r="K23" s="2">
-        <v>0</v>
-      </c>
-      <c r="L23" s="2">
-        <v>0</v>
-      </c>
-      <c r="M23" s="2">
-        <v>0</v>
-      </c>
-      <c r="N23" s="2">
-        <v>1</v>
-      </c>
-      <c r="O23" s="2">
-        <v>0</v>
-      </c>
-      <c r="P23" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q23" s="2">
-        <v>0</v>
-      </c>
-      <c r="R23" s="2">
-        <v>0</v>
-      </c>
-      <c r="S23" s="2">
-        <v>0</v>
-      </c>
-      <c r="T23" s="2">
-        <v>0</v>
-      </c>
-      <c r="U23" s="2">
-        <v>0</v>
-      </c>
-      <c r="V23" s="2">
-        <v>0</v>
-      </c>
-      <c r="W23" s="2">
-        <v>0</v>
-      </c>
-      <c r="X23" s="2">
-        <v>0</v>
-      </c>
-      <c r="Y23" s="2">
-        <v>0</v>
-      </c>
-      <c r="Z23" s="2">
-        <v>0</v>
-      </c>
-      <c r="AA23" s="2">
-        <v>0</v>
-      </c>
-      <c r="AB23" s="2">
-        <v>0</v>
-      </c>
-      <c r="AC23" s="2">
-        <v>0</v>
-      </c>
-      <c r="AD23" s="2">
-        <v>0</v>
-      </c>
-      <c r="AE23" s="2">
-        <v>1</v>
-      </c>
-      <c r="AF23" s="2">
-        <v>0</v>
-      </c>
-      <c r="AG23" s="2">
-        <v>0</v>
-      </c>
-      <c r="AH23" s="2">
-        <v>0</v>
-      </c>
-      <c r="AI23" s="2">
-        <v>0</v>
-      </c>
-      <c r="AJ23" s="2">
-        <v>0</v>
-      </c>
-      <c r="AK23" s="2">
-        <v>0</v>
-      </c>
-      <c r="AL23" s="2">
-        <v>0</v>
-      </c>
       <c r="AM23" s="2">
         <v>0</v>
       </c>
       <c r="AN23" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AO23" s="2">
         <v>0</v>
@@ -3585,7 +3585,7 @@
         <v>0</v>
       </c>
       <c r="F24" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G24" s="2">
         <v>0</v>
@@ -3603,10 +3603,10 @@
         <v>0</v>
       </c>
       <c r="L24" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M24" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N24" s="2">
         <v>0</v>
@@ -3621,7 +3621,7 @@
         <v>0</v>
       </c>
       <c r="R24" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S24" s="2">
         <v>0</v>
@@ -3642,7 +3642,7 @@
         <v>0</v>
       </c>
       <c r="Y24" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z24" s="2">
         <v>0</v>
@@ -3657,10 +3657,10 @@
         <v>0</v>
       </c>
       <c r="AD24" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE24" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF24" s="2">
         <v>0</v>
@@ -3678,7 +3678,7 @@
         <v>0</v>
       </c>
       <c r="AK24" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AL24" s="2">
         <v>0</v>
@@ -3704,7 +3704,7 @@
         <v>0</v>
       </c>
       <c r="C25" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D25" s="2">
         <v>0</v>
@@ -3722,10 +3722,10 @@
         <v>1</v>
       </c>
       <c r="I25" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J25" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K25" s="2">
         <v>0</v>
@@ -3794,10 +3794,10 @@
         <v>0</v>
       </c>
       <c r="AG25" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH25" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI25" s="2">
         <v>1</v>
@@ -3815,7 +3815,7 @@
         <v>0</v>
       </c>
       <c r="AN25" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AO25" s="2">
         <v>0</v>
@@ -3829,124 +3829,124 @@
         <v>65</v>
       </c>
       <c r="B26" s="2">
+        <v>0</v>
+      </c>
+      <c r="C26" s="2">
+        <v>0</v>
+      </c>
+      <c r="D26" s="2">
+        <v>1</v>
+      </c>
+      <c r="E26" s="2">
+        <v>0</v>
+      </c>
+      <c r="F26" s="2">
+        <v>0</v>
+      </c>
+      <c r="G26" s="2">
+        <v>0</v>
+      </c>
+      <c r="H26" s="2">
+        <v>0</v>
+      </c>
+      <c r="I26" s="2">
+        <v>0</v>
+      </c>
+      <c r="J26" s="2">
+        <v>0</v>
+      </c>
+      <c r="K26" s="2">
+        <v>0</v>
+      </c>
+      <c r="L26" s="2">
+        <v>0</v>
+      </c>
+      <c r="M26" s="2">
+        <v>0</v>
+      </c>
+      <c r="N26" s="2">
+        <v>0</v>
+      </c>
+      <c r="O26" s="2">
+        <v>0</v>
+      </c>
+      <c r="P26" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q26" s="2">
+        <v>0</v>
+      </c>
+      <c r="R26" s="2">
+        <v>0</v>
+      </c>
+      <c r="S26" s="2">
+        <v>0</v>
+      </c>
+      <c r="T26" s="2">
+        <v>0</v>
+      </c>
+      <c r="U26" s="2">
+        <v>0</v>
+      </c>
+      <c r="V26" s="2">
+        <v>0</v>
+      </c>
+      <c r="W26" s="2">
+        <v>0</v>
+      </c>
+      <c r="X26" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y26" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z26" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA26" s="2">
+        <v>1</v>
+      </c>
+      <c r="AB26" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC26" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD26" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE26" s="2">
+        <v>0</v>
+      </c>
+      <c r="AF26" s="2">
+        <v>0</v>
+      </c>
+      <c r="AG26" s="2">
+        <v>0</v>
+      </c>
+      <c r="AH26" s="2">
+        <v>0</v>
+      </c>
+      <c r="AI26" s="2">
+        <v>0</v>
+      </c>
+      <c r="AJ26" s="2">
+        <v>0</v>
+      </c>
+      <c r="AK26" s="2">
+        <v>0</v>
+      </c>
+      <c r="AL26" s="2">
+        <v>0</v>
+      </c>
+      <c r="AM26" s="2">
+        <v>0</v>
+      </c>
+      <c r="AN26" s="2">
+        <v>0</v>
+      </c>
+      <c r="AO26" s="2">
         <v>3</v>
-      </c>
-      <c r="C26" s="2">
-        <v>0</v>
-      </c>
-      <c r="D26" s="2">
-        <v>0</v>
-      </c>
-      <c r="E26" s="2">
-        <v>0</v>
-      </c>
-      <c r="F26" s="2">
-        <v>0</v>
-      </c>
-      <c r="G26" s="2">
-        <v>0</v>
-      </c>
-      <c r="H26" s="2">
-        <v>0</v>
-      </c>
-      <c r="I26" s="2">
-        <v>0</v>
-      </c>
-      <c r="J26" s="2">
-        <v>0</v>
-      </c>
-      <c r="K26" s="2">
-        <v>0</v>
-      </c>
-      <c r="L26" s="2">
-        <v>0</v>
-      </c>
-      <c r="M26" s="2">
-        <v>0</v>
-      </c>
-      <c r="N26" s="2">
-        <v>0</v>
-      </c>
-      <c r="O26" s="2">
-        <v>0</v>
-      </c>
-      <c r="P26" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q26" s="2">
-        <v>0</v>
-      </c>
-      <c r="R26" s="2">
-        <v>0</v>
-      </c>
-      <c r="S26" s="2">
-        <v>0</v>
-      </c>
-      <c r="T26" s="2">
-        <v>0</v>
-      </c>
-      <c r="U26" s="2">
-        <v>0</v>
-      </c>
-      <c r="V26" s="2">
-        <v>0</v>
-      </c>
-      <c r="W26" s="2">
-        <v>0</v>
-      </c>
-      <c r="X26" s="2">
-        <v>0</v>
-      </c>
-      <c r="Y26" s="2">
-        <v>0</v>
-      </c>
-      <c r="Z26" s="2">
-        <v>0</v>
-      </c>
-      <c r="AA26" s="2">
-        <v>0</v>
-      </c>
-      <c r="AB26" s="2">
-        <v>0</v>
-      </c>
-      <c r="AC26" s="2">
-        <v>0</v>
-      </c>
-      <c r="AD26" s="2">
-        <v>0</v>
-      </c>
-      <c r="AE26" s="2">
-        <v>0</v>
-      </c>
-      <c r="AF26" s="2">
-        <v>0</v>
-      </c>
-      <c r="AG26" s="2">
-        <v>0</v>
-      </c>
-      <c r="AH26" s="2">
-        <v>0</v>
-      </c>
-      <c r="AI26" s="2">
-        <v>0</v>
-      </c>
-      <c r="AJ26" s="2">
-        <v>0</v>
-      </c>
-      <c r="AK26" s="2">
-        <v>0</v>
-      </c>
-      <c r="AL26" s="2">
-        <v>0</v>
-      </c>
-      <c r="AM26" s="2">
-        <v>1</v>
-      </c>
-      <c r="AN26" s="2">
-        <v>0</v>
-      </c>
-      <c r="AO26" s="2">
-        <v>0</v>
       </c>
       <c r="AP26" s="2">
         <v>5</v>
@@ -4005,28 +4005,28 @@
         <v>0</v>
       </c>
       <c r="R27" s="2">
+        <v>0</v>
+      </c>
+      <c r="S27" s="2">
+        <v>0</v>
+      </c>
+      <c r="T27" s="2">
+        <v>0</v>
+      </c>
+      <c r="U27" s="2">
+        <v>0</v>
+      </c>
+      <c r="V27" s="2">
+        <v>1</v>
+      </c>
+      <c r="W27" s="2">
+        <v>0</v>
+      </c>
+      <c r="X27" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y27" s="2">
         <v>4</v>
-      </c>
-      <c r="S27" s="2">
-        <v>0</v>
-      </c>
-      <c r="T27" s="2">
-        <v>0</v>
-      </c>
-      <c r="U27" s="2">
-        <v>1</v>
-      </c>
-      <c r="V27" s="2">
-        <v>0</v>
-      </c>
-      <c r="W27" s="2">
-        <v>0</v>
-      </c>
-      <c r="X27" s="2">
-        <v>0</v>
-      </c>
-      <c r="Y27" s="2">
-        <v>0</v>
       </c>
       <c r="Z27" s="2">
         <v>0</v>
@@ -4091,7 +4091,7 @@
         <v>0</v>
       </c>
       <c r="D28" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E28" s="2">
         <v>0</v>
@@ -4106,7 +4106,7 @@
         <v>0</v>
       </c>
       <c r="I28" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J28" s="2">
         <v>0</v>
@@ -4121,10 +4121,10 @@
         <v>0</v>
       </c>
       <c r="N28" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O28" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P28" s="2">
         <v>0</v>
@@ -4163,10 +4163,10 @@
         <v>0</v>
       </c>
       <c r="AB28" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC28" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD28" s="2">
         <v>0</v>
@@ -4181,7 +4181,7 @@
         <v>0</v>
       </c>
       <c r="AH28" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI28" s="2">
         <v>0</v>
@@ -4196,7 +4196,7 @@
         <v>0</v>
       </c>
       <c r="AM28" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN28" s="2">
         <v>0</v>
@@ -4213,7 +4213,7 @@
         <v>68</v>
       </c>
       <c r="B29" s="2">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C29" s="2">
         <v>0</v>
@@ -4330,7 +4330,7 @@
         <v>0</v>
       </c>
       <c r="AO29" s="2">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AP29" s="2">
         <v>4</v>
@@ -4383,7 +4383,7 @@
         <v>0</v>
       </c>
       <c r="P30" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q30" s="2">
         <v>0</v>
@@ -4392,7 +4392,7 @@
         <v>0</v>
       </c>
       <c r="S30" s="2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="T30" s="2">
         <v>0</v>
@@ -4407,7 +4407,7 @@
         <v>0</v>
       </c>
       <c r="X30" s="2">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="Y30" s="2">
         <v>0</v>
@@ -4416,7 +4416,7 @@
         <v>0</v>
       </c>
       <c r="AA30" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB30" s="2">
         <v>0</v>
@@ -4472,7 +4472,7 @@
         <v>0</v>
       </c>
       <c r="C31" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D31" s="2">
         <v>0</v>
@@ -4490,7 +4490,7 @@
         <v>0</v>
       </c>
       <c r="I31" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J31" s="2">
         <v>0</v>
@@ -4505,7 +4505,7 @@
         <v>0</v>
       </c>
       <c r="N31" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O31" s="2">
         <v>0</v>
@@ -4550,7 +4550,7 @@
         <v>0</v>
       </c>
       <c r="AC31" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD31" s="2">
         <v>0</v>
@@ -4565,7 +4565,7 @@
         <v>0</v>
       </c>
       <c r="AH31" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI31" s="2">
         <v>0</v>
@@ -4583,7 +4583,7 @@
         <v>0</v>
       </c>
       <c r="AN31" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AO31" s="2">
         <v>0</v>
@@ -4600,7 +4600,7 @@
         <v>0</v>
       </c>
       <c r="C32" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D32" s="2">
         <v>0</v>
@@ -4615,7 +4615,7 @@
         <v>0</v>
       </c>
       <c r="H32" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I32" s="2">
         <v>0</v>
@@ -4627,7 +4627,7 @@
         <v>0</v>
       </c>
       <c r="L32" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M32" s="2">
         <v>0</v>
@@ -4684,7 +4684,7 @@
         <v>0</v>
       </c>
       <c r="AE32" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF32" s="2">
         <v>0</v>
@@ -4696,7 +4696,7 @@
         <v>0</v>
       </c>
       <c r="AI32" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ32" s="2">
         <v>0</v>
@@ -4711,7 +4711,7 @@
         <v>0</v>
       </c>
       <c r="AN32" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AO32" s="2">
         <v>0</v>
@@ -4728,7 +4728,7 @@
         <v>0</v>
       </c>
       <c r="C33" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D33" s="2">
         <v>0</v>
@@ -4755,7 +4755,7 @@
         <v>0</v>
       </c>
       <c r="L33" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M33" s="2">
         <v>0</v>
@@ -4773,7 +4773,7 @@
         <v>0</v>
       </c>
       <c r="R33" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S33" s="2">
         <v>0</v>
@@ -4794,7 +4794,7 @@
         <v>0</v>
       </c>
       <c r="Y33" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z33" s="2">
         <v>0</v>
@@ -4812,7 +4812,7 @@
         <v>0</v>
       </c>
       <c r="AE33" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF33" s="2">
         <v>0</v>
@@ -4839,7 +4839,7 @@
         <v>0</v>
       </c>
       <c r="AN33" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AO33" s="2">
         <v>0</v>
@@ -4856,7 +4856,7 @@
         <v>0</v>
       </c>
       <c r="C34" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D34" s="2">
         <v>0</v>
@@ -4871,7 +4871,7 @@
         <v>0</v>
       </c>
       <c r="H34" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I34" s="2">
         <v>0</v>
@@ -4892,7 +4892,7 @@
         <v>0</v>
       </c>
       <c r="O34" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P34" s="2">
         <v>0</v>
@@ -4931,7 +4931,7 @@
         <v>0</v>
       </c>
       <c r="AB34" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC34" s="2">
         <v>0</v>
@@ -4952,7 +4952,7 @@
         <v>0</v>
       </c>
       <c r="AI34" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ34" s="2">
         <v>0</v>
@@ -4967,7 +4967,7 @@
         <v>0</v>
       </c>
       <c r="AN34" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AO34" s="2">
         <v>0</v>
@@ -4981,10 +4981,10 @@
         <v>74</v>
       </c>
       <c r="B35" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C35" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D35" s="2">
         <v>0</v>
@@ -5095,10 +5095,10 @@
         <v>0</v>
       </c>
       <c r="AN35" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AO35" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AP35" s="2">
         <v>2</v>
@@ -5115,112 +5115,112 @@
         <v>0</v>
       </c>
       <c r="D36" s="2">
+        <v>0</v>
+      </c>
+      <c r="E36" s="2">
+        <v>0</v>
+      </c>
+      <c r="F36" s="2">
+        <v>0</v>
+      </c>
+      <c r="G36" s="2">
+        <v>0</v>
+      </c>
+      <c r="H36" s="2">
+        <v>0</v>
+      </c>
+      <c r="I36" s="2">
+        <v>0</v>
+      </c>
+      <c r="J36" s="2">
+        <v>0</v>
+      </c>
+      <c r="K36" s="2">
+        <v>0</v>
+      </c>
+      <c r="L36" s="2">
+        <v>0</v>
+      </c>
+      <c r="M36" s="2">
+        <v>0</v>
+      </c>
+      <c r="N36" s="2">
+        <v>0</v>
+      </c>
+      <c r="O36" s="2">
+        <v>0</v>
+      </c>
+      <c r="P36" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q36" s="2">
+        <v>0</v>
+      </c>
+      <c r="R36" s="2">
+        <v>0</v>
+      </c>
+      <c r="S36" s="2">
+        <v>0</v>
+      </c>
+      <c r="T36" s="2">
+        <v>0</v>
+      </c>
+      <c r="U36" s="2">
+        <v>0</v>
+      </c>
+      <c r="V36" s="2">
+        <v>0</v>
+      </c>
+      <c r="W36" s="2">
+        <v>0</v>
+      </c>
+      <c r="X36" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y36" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z36" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA36" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB36" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC36" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD36" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE36" s="2">
+        <v>0</v>
+      </c>
+      <c r="AF36" s="2">
+        <v>0</v>
+      </c>
+      <c r="AG36" s="2">
+        <v>0</v>
+      </c>
+      <c r="AH36" s="2">
+        <v>0</v>
+      </c>
+      <c r="AI36" s="2">
+        <v>0</v>
+      </c>
+      <c r="AJ36" s="2">
+        <v>0</v>
+      </c>
+      <c r="AK36" s="2">
+        <v>0</v>
+      </c>
+      <c r="AL36" s="2">
+        <v>0</v>
+      </c>
+      <c r="AM36" s="2">
         <v>2</v>
-      </c>
-      <c r="E36" s="2">
-        <v>0</v>
-      </c>
-      <c r="F36" s="2">
-        <v>0</v>
-      </c>
-      <c r="G36" s="2">
-        <v>0</v>
-      </c>
-      <c r="H36" s="2">
-        <v>0</v>
-      </c>
-      <c r="I36" s="2">
-        <v>0</v>
-      </c>
-      <c r="J36" s="2">
-        <v>0</v>
-      </c>
-      <c r="K36" s="2">
-        <v>0</v>
-      </c>
-      <c r="L36" s="2">
-        <v>0</v>
-      </c>
-      <c r="M36" s="2">
-        <v>0</v>
-      </c>
-      <c r="N36" s="2">
-        <v>0</v>
-      </c>
-      <c r="O36" s="2">
-        <v>0</v>
-      </c>
-      <c r="P36" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q36" s="2">
-        <v>0</v>
-      </c>
-      <c r="R36" s="2">
-        <v>0</v>
-      </c>
-      <c r="S36" s="2">
-        <v>0</v>
-      </c>
-      <c r="T36" s="2">
-        <v>0</v>
-      </c>
-      <c r="U36" s="2">
-        <v>0</v>
-      </c>
-      <c r="V36" s="2">
-        <v>0</v>
-      </c>
-      <c r="W36" s="2">
-        <v>0</v>
-      </c>
-      <c r="X36" s="2">
-        <v>0</v>
-      </c>
-      <c r="Y36" s="2">
-        <v>0</v>
-      </c>
-      <c r="Z36" s="2">
-        <v>0</v>
-      </c>
-      <c r="AA36" s="2">
-        <v>0</v>
-      </c>
-      <c r="AB36" s="2">
-        <v>0</v>
-      </c>
-      <c r="AC36" s="2">
-        <v>0</v>
-      </c>
-      <c r="AD36" s="2">
-        <v>0</v>
-      </c>
-      <c r="AE36" s="2">
-        <v>0</v>
-      </c>
-      <c r="AF36" s="2">
-        <v>0</v>
-      </c>
-      <c r="AG36" s="2">
-        <v>0</v>
-      </c>
-      <c r="AH36" s="2">
-        <v>0</v>
-      </c>
-      <c r="AI36" s="2">
-        <v>0</v>
-      </c>
-      <c r="AJ36" s="2">
-        <v>0</v>
-      </c>
-      <c r="AK36" s="2">
-        <v>0</v>
-      </c>
-      <c r="AL36" s="2">
-        <v>0</v>
-      </c>
-      <c r="AM36" s="2">
-        <v>0</v>
       </c>
       <c r="AN36" s="2">
         <v>0</v>
@@ -5261,13 +5261,13 @@
         <v>0</v>
       </c>
       <c r="J37" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K37" s="2">
         <v>0</v>
       </c>
       <c r="L37" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M37" s="2">
         <v>0</v>
@@ -5324,13 +5324,13 @@
         <v>0</v>
       </c>
       <c r="AE37" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF37" s="2">
         <v>0</v>
       </c>
       <c r="AG37" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH37" s="2">
         <v>0</v>
@@ -5368,7 +5368,7 @@
         <v>0</v>
       </c>
       <c r="C38" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D38" s="2">
         <v>0</v>
@@ -5377,7 +5377,7 @@
         <v>0</v>
       </c>
       <c r="F38" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G38" s="2">
         <v>0</v>
@@ -5470,7 +5470,7 @@
         <v>0</v>
       </c>
       <c r="AK38" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL38" s="2">
         <v>0</v>
@@ -5479,7 +5479,7 @@
         <v>0</v>
       </c>
       <c r="AN38" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AO38" s="2">
         <v>0</v>
@@ -5541,7 +5541,7 @@
         <v>0</v>
       </c>
       <c r="R39" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S39" s="2">
         <v>0</v>
@@ -5562,7 +5562,7 @@
         <v>0</v>
       </c>
       <c r="Y39" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z39" s="2">
         <v>0</v>
@@ -5624,7 +5624,7 @@
         <v>0</v>
       </c>
       <c r="C40" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D40" s="2">
         <v>0</v>
@@ -5735,7 +5735,7 @@
         <v>0</v>
       </c>
       <c r="AN40" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AO40" s="2">
         <v>0</v>
@@ -5761,7 +5761,7 @@
         <v>0</v>
       </c>
       <c r="F41" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G41" s="2">
         <v>0</v>
@@ -5854,7 +5854,7 @@
         <v>0</v>
       </c>
       <c r="AK41" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL41" s="2">
         <v>0</v>
@@ -5898,7 +5898,7 @@
         <v>0</v>
       </c>
       <c r="I42" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J42" s="2">
         <v>0</v>
@@ -5973,7 +5973,7 @@
         <v>0</v>
       </c>
       <c r="AH42" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI42" s="2">
         <v>0</v>
@@ -6062,10 +6062,10 @@
         <v>0</v>
       </c>
       <c r="U43" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V43" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W43" s="2">
         <v>0</v>

</xml_diff>